<commit_message>
FSM for laval, updated modesl, included belt anim
Full boiler&engine state machine, laval SM with collab trigger, laval
system working, laval belt texture animation. FSM still separate for two
machines. Updated Factory and Machinery to automate start/stop operation
and wheels/belts opeartion (now in separate dictionaries).
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="175">
   <si>
     <t>Current State</t>
   </si>
@@ -443,9 +443,6 @@
     <t>i/Great! The boiler's furnace is being loaded with coal</t>
   </si>
   <si>
-    <t>Void</t>
-  </si>
-  <si>
     <t>entry</t>
   </si>
   <si>
@@ -467,34 +464,97 @@
     <t>Good! You can now ignite the boiler again by loading  more coal</t>
   </si>
   <si>
-    <t>dropping_pressure_1500psi</t>
-  </si>
-  <si>
     <t>a/Danger! Boiler pressure is very low (1,500 psi) and machines are malfunctioning</t>
   </si>
   <si>
     <t>a/Beware! Boiler pressure is marginally low (3,000 psi) for normal operation</t>
   </si>
   <si>
-    <t>stopping_engine; dropping_pressure_0psi</t>
-  </si>
-  <si>
     <t>You need to turn steam supply off to prevent machine malfunction</t>
   </si>
   <si>
     <t>match_coalfurnace</t>
   </si>
   <si>
-    <t>Fire is necessary to light the coals and start the fire</t>
-  </si>
-  <si>
-    <t>error_boiler; dropping_pressure_3000psi</t>
-  </si>
-  <si>
-    <t>increasing_pressure_4500psi</t>
-  </si>
-  <si>
     <t>starting_engine; starting_timer</t>
+  </si>
+  <si>
+    <t>dropping_pressure_1500psi; dying_away_fire</t>
+  </si>
+  <si>
+    <t>stopping_engine; dropping_pressure_0psi; exhausting_fire</t>
+  </si>
+  <si>
+    <t>Nice! This valve provides steam from the boiler to the steam engine</t>
+  </si>
+  <si>
+    <t>error1_boiler; dropping_pressure_3000psi</t>
+  </si>
+  <si>
+    <t>stopping_timer; increasing_pressure_4500psi; error0_boiler</t>
+  </si>
+  <si>
+    <t>error1_boiler</t>
+  </si>
+  <si>
+    <t>increasing_pressure_4500psi; error0_boiler</t>
+  </si>
+  <si>
+    <t>belt_powerWheel</t>
+  </si>
+  <si>
+    <t>Good job! These belts are used to provide motion from the engine to the machinery</t>
+  </si>
+  <si>
+    <t>belt_wheel</t>
+  </si>
+  <si>
+    <t>You need someone else to loosen the Laval's power wheel and stretch the belt</t>
+  </si>
+  <si>
+    <t>wrench_powerWheel</t>
+  </si>
+  <si>
+    <t>Laval-belt-off</t>
+  </si>
+  <si>
+    <t>Laval-belt-on</t>
+  </si>
+  <si>
+    <t>You need someone else to place and stretch the belt on the driving wheel side</t>
+  </si>
+  <si>
+    <t>You should place the belt on the side of the driving wheel first</t>
+  </si>
+  <si>
+    <t>wrench_wheel</t>
+  </si>
+  <si>
+    <t>You can't loosen the driving wheel</t>
+  </si>
+  <si>
+    <t>i/Great! The Laval separator is ready to be set in motion</t>
+  </si>
+  <si>
+    <t>belt_wheel, wrench_powerWheel</t>
+  </si>
+  <si>
+    <t>attaching_belt*</t>
+  </si>
+  <si>
+    <t>a/The olive press does not have power!</t>
+  </si>
+  <si>
+    <t>a/A belt is missing from one of the machines</t>
+  </si>
+  <si>
+    <t>detaching_laval_belt; error1_lavalL</t>
+  </si>
+  <si>
+    <t>Matches was one of the ways to light the coals and start the fire</t>
+  </si>
+  <si>
+    <t>hand_coal, hand_coal</t>
   </si>
 </sst>
 </file>
@@ -676,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -708,6 +768,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1995,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2006,12 +2067,12 @@
     <col min="1" max="2" width="16.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="17" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="74.85546875" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2030,11 +2091,8 @@
       <c r="F1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
@@ -2042,16 +2100,16 @@
         <v>135</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>154</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2059,19 +2117,17 @@
         <v>135</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>174</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="5"/>
       <c r="F3" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2082,14 +2138,12 @@
         <v>109</v>
       </c>
       <c r="D4" s="4"/>
+      <c r="E4" s="5"/>
       <c r="F4" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
@@ -2097,7 +2151,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="27" t="s">
@@ -2106,11 +2160,8 @@
       <c r="F5" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="G5" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2121,14 +2172,12 @@
         <v>3</v>
       </c>
       <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -2143,11 +2192,8 @@
       <c r="F7" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2155,7 +2201,7 @@
         <v>135</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>14</v>
@@ -2164,13 +2210,10 @@
         <v>113</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>14</v>
       </c>
@@ -2178,20 +2221,17 @@
         <v>135</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="27" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2205,11 +2245,8 @@
       <c r="F10" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -2217,17 +2254,14 @@
         <v>135</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" s="4"/>
       <c r="F11" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -2243,12 +2277,11 @@
       <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>11</v>
       </c>
@@ -2256,20 +2289,17 @@
         <v>135</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="27" t="s">
         <v>152</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="G13" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -2277,20 +2307,17 @@
         <v>135</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="5" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2298,7 +2325,7 @@
         <v>135</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>15</v>
@@ -2307,11 +2334,8 @@
         <v>21</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
@@ -2322,19 +2346,16 @@
         <v>3</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -2346,13 +2367,10 @@
       </c>
       <c r="D17" s="4"/>
       <c r="F17" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>15</v>
       </c>
@@ -2360,20 +2378,17 @@
         <v>135</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="27" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="G18" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2385,13 +2400,10 @@
       </c>
       <c r="D19" s="4"/>
       <c r="F19" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -2408,13 +2420,10 @@
         <v>17</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>111</v>
       </c>
@@ -2422,20 +2431,17 @@
         <v>135</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="G21" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>111</v>
       </c>
@@ -2449,11 +2455,8 @@
       <c r="F22" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>111</v>
       </c>
@@ -2467,11 +2470,8 @@
       <c r="F23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>111</v>
       </c>
@@ -2485,30 +2485,114 @@
         <v>11</v>
       </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+    </row>
+    <row r="25" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mill animations almost ready
SM updated with right mill acitons/states and 1 sack, except:
- sack animation still needs refinement (WorldViz support)
- some models are missing (paste pouring, water can, straight hatch,
fake hole, pulp texture)
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="287">
   <si>
     <t>Current State</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>turning_valve_on</t>
-  </si>
-  <si>
-    <t>10_mins_later</t>
   </si>
   <si>
     <t>Μηχάνημα</t>
@@ -341,12 +338,6 @@
     <t>You are shoveling coal in the boiler, which is necessary for its operation</t>
   </si>
   <si>
-    <t>15_mins_later</t>
-  </si>
-  <si>
-    <t>20_mins_later</t>
-  </si>
-  <si>
     <t>Steam supply is already on, you should better not turn off the engine!</t>
   </si>
   <si>
@@ -474,9 +465,6 @@
   </si>
   <si>
     <t>Machine States</t>
-  </si>
-  <si>
-    <t>boiler/idle; engine/idle; lavalL/belt-off</t>
   </si>
   <si>
     <t>factory/start</t>
@@ -881,16 +869,151 @@
     <t>millR/loaded</t>
   </si>
   <si>
-    <t>hand_sack</t>
-  </si>
-  <si>
-    <t>loading_olives</t>
-  </si>
-  <si>
-    <t>i//Good! You have emptied a whole sack (100 lb) into the mill</t>
-  </si>
-  <si>
-    <t>starting_crash</t>
+    <t>hand_sack1R</t>
+  </si>
+  <si>
+    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/empty</t>
+  </si>
+  <si>
+    <t>error1_millR</t>
+  </si>
+  <si>
+    <t>loading_mill1R*; error0_millR</t>
+  </si>
+  <si>
+    <t>millR/loading</t>
+  </si>
+  <si>
+    <t>You have emptied a whole sack of olives (100 lb) into the mill</t>
+  </si>
+  <si>
+    <t>i//Good! The right mill is has started crashing the olives</t>
+  </si>
+  <si>
+    <t>hand_sack2R</t>
+  </si>
+  <si>
+    <t>paste-thick</t>
+  </si>
+  <si>
+    <t>15-mins-later</t>
+  </si>
+  <si>
+    <t>20-mins-later</t>
+  </si>
+  <si>
+    <t>10-mins-later</t>
+  </si>
+  <si>
+    <t>There are enough olives in the mill already</t>
+  </si>
+  <si>
+    <t>paste-ready</t>
+  </si>
+  <si>
+    <t>millR/paste-ready</t>
+  </si>
+  <si>
+    <t>millR/paste-thick</t>
+  </si>
+  <si>
+    <t>water_paste</t>
+  </si>
+  <si>
+    <t>a/millR/The paste is too thick and needs to be diluted</t>
+  </si>
+  <si>
+    <t>millR/pulp</t>
+  </si>
+  <si>
+    <t>There is no need to put water in the paste, yet</t>
+  </si>
+  <si>
+    <t>You are pooring water in the paste to prevent it from becoming too thick</t>
+  </si>
+  <si>
+    <t>hand_hatch</t>
+  </si>
+  <si>
+    <t>Good, you are emptying the paste in the pulp tank</t>
+  </si>
+  <si>
+    <t>paste-hot</t>
+  </si>
+  <si>
+    <t>a/millR/The paste is ready and needs to be removed from the right mill</t>
+  </si>
+  <si>
+    <t>a/millR/The paste has become too hot and needs to be removed immediately!</t>
+  </si>
+  <si>
+    <t>i//Good job! The olive paste should be diluted quite often with water</t>
+  </si>
+  <si>
+    <t>The paste is liquid enough, no need for extra water</t>
+  </si>
+  <si>
+    <t>a/millR/The paste in the right mill is extremely thick and will be wasted!</t>
+  </si>
+  <si>
+    <t>hand_tank</t>
+  </si>
+  <si>
+    <t>You need to move the paste to the loading table before you load more olives in the mill</t>
+  </si>
+  <si>
+    <t>timerM1_readyR</t>
+  </si>
+  <si>
+    <t>paste-dilute</t>
+  </si>
+  <si>
+    <t>The paste is ready and does not need any more dilution</t>
+  </si>
+  <si>
+    <t>a/millR/Too bad! The paste got too hot and is now wasted!</t>
+  </si>
+  <si>
+    <t>paste-wasted</t>
+  </si>
+  <si>
+    <t>a/millR/Too bad! The paste got too thick and hot and is now wasted!</t>
+  </si>
+  <si>
+    <t>starting_crashR; timerM1_diluteR</t>
+  </si>
+  <si>
+    <t>error1_millR; timerM1_thickR; timerM1_wastedR</t>
+  </si>
+  <si>
+    <t>error1_millR; timerM1_hotR; timerM1_wastedR</t>
+  </si>
+  <si>
+    <t>error0_millR; timerM0_thickR; timerM0_wastedR</t>
+  </si>
+  <si>
+    <t>error0_millR; timerM0_hotR; timerM0_wastedR</t>
+  </si>
+  <si>
+    <t>pouring_pasteR</t>
+  </si>
+  <si>
+    <t>wasting_pasteR</t>
+  </si>
+  <si>
+    <t>millR/pouring</t>
+  </si>
+  <si>
+    <t>anim-finished</t>
+  </si>
+  <si>
+    <t>millR/tank-full</t>
+  </si>
+  <si>
+    <t>i//Nice! The paste in the right mill is ready to be tranfered to the loading table</t>
+  </si>
+  <si>
+    <t>Good! You are moving the paste to the loading table</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1156,6 +1279,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1472,213 +1596,213 @@
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="10">
         <v>1</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="15">
         <v>1</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="15">
         <v>2</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="16">
         <v>2</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>4</v>
@@ -1687,349 +1811,349 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="15">
         <v>2</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
       </c>
       <c r="D18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="F18" s="15">
         <v>2</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="14" t="s">
         <v>55</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="15">
         <v>1</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" s="15">
         <v>2</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2058,39 +2182,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F2" s="37">
         <v>7.2916666666666671E-2</v>
@@ -2098,16 +2222,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F3" s="37">
         <v>3.125E-2</v>
@@ -2115,27 +2239,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F5" s="37">
         <v>4.1666666666666664E-2</v>
@@ -2143,27 +2267,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="D7" t="s">
-        <v>188</v>
-      </c>
       <c r="E7" s="38" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F7" s="42">
         <v>3.4722222222222224E-2</v>
@@ -2171,41 +2295,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
         <v>184</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="D8" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" t="s">
         <v>184</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C10" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="D10" s="40" t="s">
-        <v>207</v>
-      </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F10" s="37">
         <v>0.10416666666666667</v>
@@ -2213,28 +2337,28 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>205</v>
-      </c>
       <c r="D11" s="40" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="D12" s="40" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F12" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2242,16 +2366,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F13" s="37">
         <v>6.25E-2</v>
@@ -2259,27 +2383,27 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E15" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F15" s="37">
         <v>3.4722222222222224E-2</v>
@@ -2287,19 +2411,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16" s="37" t="s">
         <v>219</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>223</v>
       </c>
       <c r="F16" s="37">
         <v>7.2916666666666671E-2</v>
@@ -2307,16 +2431,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F17" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2324,14 +2448,14 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F18" s="37">
         <v>6.5972222222222224E-2</v>
@@ -2339,27 +2463,27 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>207</v>
+      </c>
+      <c r="B21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="36" t="s">
         <v>211</v>
       </c>
-      <c r="B21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>215</v>
-      </c>
       <c r="D21" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F21" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2367,44 +2491,44 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D22" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D23" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="D24" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="C24" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>221</v>
-      </c>
       <c r="E24" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F24" s="37">
         <v>9.7222222222222224E-2</v>
@@ -2412,16 +2536,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="D25" t="s">
         <v>233</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>234</v>
-      </c>
-      <c r="D25" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2437,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2458,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2467,651 +2591,1003 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="22"/>
       <c r="E7" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D8" s="3"/>
       <c r="F8" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" s="3"/>
       <c r="F9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>249</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>103</v>
+        <v>247</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>104</v>
+        <v>248</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="F15" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D16" s="28"/>
       <c r="F16" s="26" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4"/>
       <c r="F18" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
       <c r="F20" s="26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="3"/>
       <c r="F22" s="26" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="3"/>
       <c r="F28" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D29" s="28"/>
       <c r="F29" s="26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="E39" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="F40" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E41" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="22"/>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>245</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="F45" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="E48" s="43"/>
+      <c r="F48" s="26" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E55" s="43"/>
+      <c r="F55" s="26" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="E56" s="43"/>
+      <c r="F56" s="26" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="B57" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>281</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3122,10 +3598,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3140,65 +3616,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>148</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished mill; made loader, press interactions
millR with 2 sacks is ready (bug with paste layer)
pressR is working besides filling it up after 4th mat
loader (table) interactions working
two lavals with tanks are in place
changed belt system for lavals
updated state machine to support actions between mill-loader-press
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="345">
   <si>
     <t>Current State</t>
   </si>
@@ -501,9 +501,6 @@
   </si>
   <si>
     <t>engine/belt</t>
-  </si>
-  <si>
-    <t>hand_wheel</t>
   </si>
   <si>
     <t>LavalL/belt-on</t>
@@ -863,18 +860,9 @@
     <t>millR/empty</t>
   </si>
   <si>
-    <t>a/millR/The right mill is empty, you need to load it with olives</t>
-  </si>
-  <si>
     <t>millR/loaded</t>
   </si>
   <si>
-    <t>hand_sack1R</t>
-  </si>
-  <si>
-    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/empty</t>
-  </si>
-  <si>
     <t>error1_millR</t>
   </si>
   <si>
@@ -884,12 +872,6 @@
     <t>millR/loading</t>
   </si>
   <si>
-    <t>You have emptied a whole sack of olives (100 lb) into the mill</t>
-  </si>
-  <si>
-    <t>i//Good! The right mill is has started crashing the olives</t>
-  </si>
-  <si>
     <t>hand_sack2R</t>
   </si>
   <si>
@@ -920,9 +902,6 @@
     <t>water_paste</t>
   </si>
   <si>
-    <t>a/millR/The paste is too thick and needs to be diluted</t>
-  </si>
-  <si>
     <t>millR/pulp</t>
   </si>
   <si>
@@ -935,15 +914,9 @@
     <t>hand_hatch</t>
   </si>
   <si>
-    <t>Good, you are emptying the paste in the pulp tank</t>
-  </si>
-  <si>
     <t>paste-hot</t>
   </si>
   <si>
-    <t>a/millR/The paste is ready and needs to be removed from the right mill</t>
-  </si>
-  <si>
     <t>a/millR/The paste has become too hot and needs to be removed immediately!</t>
   </si>
   <si>
@@ -953,9 +926,6 @@
     <t>The paste is liquid enough, no need for extra water</t>
   </si>
   <si>
-    <t>a/millR/The paste in the right mill is extremely thick and will be wasted!</t>
-  </si>
-  <si>
     <t>hand_tank</t>
   </si>
   <si>
@@ -971,9 +941,6 @@
     <t>The paste is ready and does not need any more dilution</t>
   </si>
   <si>
-    <t>a/millR/Too bad! The paste got too hot and is now wasted!</t>
-  </si>
-  <si>
     <t>paste-wasted</t>
   </si>
   <si>
@@ -1010,17 +977,224 @@
     <t>millR/tank-full</t>
   </si>
   <si>
-    <t>i//Nice! The paste in the right mill is ready to be tranfered to the loading table</t>
-  </si>
-  <si>
     <t>Good! You are moving the paste to the loading table</t>
+  </si>
+  <si>
+    <t>hand_wheel, hand_wheel</t>
+  </si>
+  <si>
+    <t>hand_sack1R, hand_sack1R</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>* indicates that only one player executes the action, and also updates other participating players with the message</t>
+  </si>
+  <si>
+    <t>error1 = display alert on the map</t>
+  </si>
+  <si>
+    <t>error0 = eliminate the alert from map</t>
+  </si>
+  <si>
+    <t>timerM1 = start timer related to mill functionality</t>
+  </si>
+  <si>
+    <t>timerM0 = kill timer related to mill functionality</t>
+  </si>
+  <si>
+    <t>1R = the first sack of the right mill</t>
+  </si>
+  <si>
+    <t>Good teamwork! You have emptied a whole sack of olives (100 lb) into the right mill</t>
+  </si>
+  <si>
+    <t>loader/idle</t>
+  </si>
+  <si>
+    <t>hand_mat</t>
+  </si>
+  <si>
+    <t>i//Good! Mill No2 has started crashing the olives</t>
+  </si>
+  <si>
+    <t>a/millR/The paste in Mill No2 is too thick and needs to be diluted</t>
+  </si>
+  <si>
+    <t>a/millR/The paste in Mill No2 is extremely thick and will be wasted!</t>
+  </si>
+  <si>
+    <t>a/millR/The paste is ready and needs to be removed from Mill No2</t>
+  </si>
+  <si>
+    <t>a/millR/Too bad! The paste in Mill No2 got too hot and is now wasted!</t>
+  </si>
+  <si>
+    <t>i//Nice! The paste in mill No2 is ready to be tranfered to the loading table</t>
+  </si>
+  <si>
+    <t>a/millR/Mill No2 is empty, you need to load it with olives</t>
+  </si>
+  <si>
+    <t>hand_matPile</t>
+  </si>
+  <si>
+    <t>loader/mat-empty</t>
+  </si>
+  <si>
+    <t>loader/ready</t>
+  </si>
+  <si>
+    <t>can_pulp</t>
+  </si>
+  <si>
+    <t>You need to set a mat on the table first, before loading it with the paste</t>
+  </si>
+  <si>
+    <t>You are ready to load the mat with the olive paste from the big tank</t>
+  </si>
+  <si>
+    <t>canful_mat</t>
+  </si>
+  <si>
+    <t>loading_mat</t>
+  </si>
+  <si>
+    <t>You can only load one mat at a time</t>
+  </si>
+  <si>
+    <t>i//The mat is ready to be loaded to one of the presses</t>
+  </si>
+  <si>
+    <t>picking_mat</t>
+  </si>
+  <si>
+    <t>pressR/empty</t>
+  </si>
+  <si>
+    <t>pressR/idle</t>
+  </si>
+  <si>
+    <t>a/pressR/Press No2 is empty and needs to be loaded with mats full of paste</t>
+  </si>
+  <si>
+    <t>Good! You have placed a mat with olive paste on the press</t>
+  </si>
+  <si>
+    <t>pressR/loading</t>
+  </si>
+  <si>
+    <t>Good! You have placed another mat with olive paste on the press</t>
+  </si>
+  <si>
+    <t>pressR/loading2</t>
+  </si>
+  <si>
+    <t>pressR/loading3</t>
+  </si>
+  <si>
+    <t>Keep on! By placing another mat Press No2 will be automatically fully loaded</t>
+  </si>
+  <si>
+    <t>i//Each press would need to be loaded with at least 20 mats before starting up</t>
+  </si>
+  <si>
+    <t>pressR/loaded</t>
+  </si>
+  <si>
+    <t>i//This was a laborious manual task but necessary during the cold olive press process</t>
+  </si>
+  <si>
+    <t>i//Good job! You have fully loaded Press No2 and are ready to start pressing</t>
+  </si>
+  <si>
+    <t>You have picked the mat and can now load it on one of the presses</t>
+  </si>
+  <si>
+    <t>resetting_millR</t>
+  </si>
+  <si>
+    <t>error1_pressR</t>
+  </si>
+  <si>
+    <t>Good, you are emptying the paste in the mill's tank</t>
+  </si>
+  <si>
+    <t>i//Good, you're ready to start loading the mats on the presses</t>
+  </si>
+  <si>
+    <t>millR/reset</t>
+  </si>
+  <si>
+    <t>anim-finished = triggered with timer expiration</t>
+  </si>
+  <si>
+    <t>transfering_tankR</t>
+  </si>
+  <si>
+    <t>loader/ready:loader/idle; pressR/empty:pressR/idle</t>
+  </si>
+  <si>
+    <t>i//The straw mat is on the table ready to be loaded with the olive paste</t>
+  </si>
+  <si>
+    <t>serving_mat</t>
+  </si>
+  <si>
+    <t>loader/mat-full</t>
+  </si>
+  <si>
+    <t>can_mat</t>
+  </si>
+  <si>
+    <t>scooping_pulp</t>
+  </si>
+  <si>
+    <t>You don't have any olive paste in the tank to load the mat</t>
+  </si>
+  <si>
+    <t>get-pulp</t>
+  </si>
+  <si>
+    <t>getting_pulp+5</t>
+  </si>
+  <si>
+    <t>Great teamwork! You have spread out the paste on the mat</t>
+  </si>
+  <si>
+    <t>The mat is still empty, you need to load it with olive paste first before you move it to the press</t>
+  </si>
+  <si>
+    <t>The container is empty, you need to scoop some paste first from the big tank</t>
+  </si>
+  <si>
+    <t>You have loaded the can with the olive paste and are ready to lay it on the mat</t>
+  </si>
+  <si>
+    <t>mat_as_tool</t>
+  </si>
+  <si>
+    <t>You need to load the existing mat on the press before using a new mat</t>
+  </si>
+  <si>
+    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/paste-ready; loader/ready; pressR/empty</t>
+  </si>
+  <si>
+    <t>mat_tray</t>
+  </si>
+  <si>
+    <t>Keep on! By placing another mat, Press No2 will be automatically fully loaded</t>
+  </si>
+  <si>
+    <t>loading_pressR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1178,6 +1352,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1227,7 +1416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1280,6 +1469,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2182,39 +2373,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
         <v>173</v>
       </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
       <c r="C2" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F2" s="37">
         <v>7.2916666666666671E-2</v>
@@ -2222,16 +2413,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>178</v>
-      </c>
       <c r="D3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F3" s="37">
         <v>3.125E-2</v>
@@ -2239,27 +2430,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F5" s="37">
         <v>4.1666666666666664E-2</v>
@@ -2267,27 +2458,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F7" s="42">
         <v>3.4722222222222224E-2</v>
@@ -2295,41 +2486,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F10" s="37">
         <v>0.10416666666666667</v>
@@ -2337,28 +2528,28 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="40" t="s">
         <v>201</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>202</v>
       </c>
       <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>223</v>
-      </c>
       <c r="D12" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F12" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2366,16 +2557,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D13" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F13" s="37">
         <v>6.25E-2</v>
@@ -2383,27 +2574,27 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F15" s="37">
         <v>3.4722222222222224E-2</v>
@@ -2411,19 +2602,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F16" s="37">
         <v>7.2916666666666671E-2</v>
@@ -2431,16 +2622,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>215</v>
-      </c>
       <c r="E17" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F17" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2448,14 +2639,14 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="38" t="s">
         <v>226</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>227</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F18" s="37">
         <v>6.5972222222222224E-2</v>
@@ -2463,27 +2654,27 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="36" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" t="s">
-        <v>210</v>
-      </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F21" s="37">
         <v>7.9861111111111105E-2</v>
@@ -2491,44 +2682,44 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="D22" t="s">
         <v>209</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="E22" s="41" t="s">
         <v>231</v>
-      </c>
-      <c r="D22" t="s">
-        <v>210</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D23" t="s">
         <v>209</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>212</v>
-      </c>
-      <c r="D23" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C24" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="D24" s="40" t="s">
-        <v>217</v>
-      </c>
       <c r="E24" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F24" s="37">
         <v>9.7222222222222224E-2</v>
@@ -2536,16 +2727,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="s">
         <v>228</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="C25" s="36" t="s">
-        <v>230</v>
-      </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2561,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2573,11 +2764,12 @@
     <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17" style="2" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="74.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="68.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2596,8 +2788,11 @@
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>133</v>
       </c>
@@ -2611,17 +2806,20 @@
         <v>109</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>133</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="44" t="s">
         <v>122</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -2632,7 +2830,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>134</v>
       </c>
@@ -2647,17 +2845,17 @@
         <v>5</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>134</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="44" t="s">
         <v>122</v>
       </c>
       <c r="D5" s="3"/>
@@ -2666,14 +2864,14 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>134</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="44" t="s">
         <v>150</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -2686,7 +2884,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
         <v>135</v>
       </c>
@@ -2701,17 +2899,20 @@
         <v>131</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>135</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="44" t="s">
         <v>122</v>
       </c>
       <c r="D8" s="3"/>
@@ -2719,7 +2920,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>135</v>
       </c>
@@ -2734,7 +2935,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="34" t="s">
         <v>135</v>
       </c>
@@ -2742,14 +2943,14 @@
         <v>132</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>136</v>
       </c>
@@ -2764,10 +2965,10 @@
         <v>108</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>136</v>
       </c>
@@ -2775,17 +2976,17 @@
         <v>132</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="4" t="s">
         <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>136</v>
       </c>
@@ -2793,7 +2994,7 @@
         <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>124</v>
@@ -2802,10 +3003,10 @@
         <v>151</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>136</v>
       </c>
@@ -2822,10 +3023,10 @@
         <v>147</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="34" t="s">
         <v>137</v>
       </c>
@@ -2841,7 +3042,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="34" t="s">
         <v>137</v>
       </c>
@@ -2856,7 +3057,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>138</v>
       </c>
@@ -2869,7 +3070,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>138</v>
       </c>
@@ -2885,7 +3086,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19" t="s">
         <v>156</v>
       </c>
@@ -2898,7 +3099,7 @@
       <c r="D19" s="22"/>
       <c r="E19" s="25"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>156</v>
       </c>
@@ -2914,7 +3115,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>148</v>
       </c>
@@ -2927,7 +3128,7 @@
       <c r="D21" s="22"/>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>148</v>
       </c>
@@ -2942,7 +3143,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19" t="s">
         <v>139</v>
       </c>
@@ -2957,7 +3158,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
         <v>139</v>
       </c>
@@ -2977,7 +3178,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>152</v>
       </c>
@@ -2990,7 +3191,7 @@
       <c r="D25" s="22"/>
       <c r="E25" s="25"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
         <v>152</v>
       </c>
@@ -3010,7 +3211,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>140</v>
       </c>
@@ -3025,10 +3226,10 @@
         <v>130</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>140</v>
       </c>
@@ -3043,7 +3244,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
         <v>140</v>
       </c>
@@ -3058,7 +3259,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
         <v>146</v>
       </c>
@@ -3071,7 +3272,7 @@
       <c r="D30" s="22"/>
       <c r="E30" s="25"/>
     </row>
-    <row r="31" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
         <v>141</v>
       </c>
@@ -3086,30 +3287,33 @@
         <v>119</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>141</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="E32" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>141</v>
       </c>
@@ -3123,7 +3327,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>141</v>
       </c>
@@ -3137,7 +3341,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>141</v>
       </c>
@@ -3151,7 +3355,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>141</v>
       </c>
@@ -3165,7 +3369,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
         <v>142</v>
       </c>
@@ -3176,12 +3380,12 @@
         <v>100</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>132</v>
@@ -3190,9 +3394,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>132</v>
@@ -3201,35 +3405,38 @@
         <v>100</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="E40" s="4" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>132</v>
@@ -3240,24 +3447,27 @@
       <c r="D41" s="22"/>
       <c r="E41" s="25"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G42" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>132</v>
@@ -3266,59 +3476,65 @@
         <v>100</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D45" s="3"/>
       <c r="F45" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>132</v>
@@ -3327,70 +3543,70 @@
         <v>100</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="E48" s="43"/>
       <c r="F48" s="26" t="s">
-        <v>266</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E49" s="43" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F49" s="26" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>132</v>
@@ -3399,43 +3615,43 @@
         <v>100</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>248</v>
+      </c>
+      <c r="F52" s="26" t="s">
         <v>256</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="24" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>132</v>
@@ -3444,127 +3660,127 @@
         <v>100</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="26" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B55" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="E55" s="43"/>
       <c r="F55" s="26" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="26" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B56" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C56" s="26" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E56" s="43"/>
       <c r="F56" s="26" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="26" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B57" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C57" s="26" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="F57" s="26" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="D58" s="3" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C59" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="B60" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C60" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="F60" s="24" t="s">
-        <v>268</v>
+      <c r="E59" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C60" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>132</v>
@@ -3573,21 +3789,474 @@
         <v>100</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>267</v>
+        <v>257</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="F63" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="E66" s="43" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E69" s="25"/>
+      <c r="F69" s="24" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="F73" s="24" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>294</v>
+      </c>
+      <c r="D74" s="28"/>
+      <c r="F74" s="26" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B75" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C75" s="26" t="s">
         <v>286</v>
+      </c>
+      <c r="D75" s="28"/>
+      <c r="F75" s="26" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B76" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D76" s="28"/>
+      <c r="F76" s="26" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D78" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E80" s="4"/>
+      <c r="F80" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="B82" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E82" s="25"/>
+    </row>
+    <row r="83" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B83" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E83" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="25"/>
+      <c r="F85" s="24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C87" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D87" s="24"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="24" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D89" s="24"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3598,7 +4267,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -3633,7 +4302,7 @@
         <v>143</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>239</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3658,7 +4327,7 @@
         <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3669,7 +4338,7 @@
         <v>143</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3680,7 +4349,7 @@
         <v>143</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3691,7 +4360,18 @@
         <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed avatar height bug; SM for press-pump interaction; pump updated
- Fixed avatar eyheight (collision with map!)
- Replaced new pump model with reduced
- SM entries for pump-press interaction
- olive pump in place
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="400">
   <si>
     <t>Current State</t>
   </si>
@@ -350,15 +350,9 @@
     <t>match_coalfurnace</t>
   </si>
   <si>
-    <t>dropping_pressure_1500psi; dying_away_fire</t>
-  </si>
-  <si>
     <t>Nice! This valve provides steam from the boiler to the steam engine</t>
   </si>
   <si>
-    <t>error1_boiler; dropping_pressure_3000psi</t>
-  </si>
-  <si>
     <t>error1_boiler</t>
   </si>
   <si>
@@ -425,9 +419,6 @@
     <t>starting_engine</t>
   </si>
   <si>
-    <t>increasing_pressure_4500psi; starting_timer; error0_boiler</t>
-  </si>
-  <si>
     <t>MachineState</t>
   </si>
   <si>
@@ -473,9 +464,6 @@
     <t>lavalL/idle</t>
   </si>
   <si>
-    <t>stopping_timer; increasing_pressure_4500psi; renewing_fire</t>
-  </si>
-  <si>
     <t>engine/steam</t>
   </si>
   <si>
@@ -483,9 +471,6 @@
   </si>
   <si>
     <t>hand_coalfurnace</t>
-  </si>
-  <si>
-    <t>stopping_timer; dropping_pressure_0psi; exhausting_fire</t>
   </si>
   <si>
     <t>engine/ready</t>
@@ -1058,9 +1043,6 @@
     <t>canful_mat</t>
   </si>
   <si>
-    <t>loading_mat</t>
-  </si>
-  <si>
     <t>You can only load one mat at a time</t>
   </si>
   <si>
@@ -1085,33 +1067,18 @@
     <t>pressR/loading</t>
   </si>
   <si>
-    <t>Good! You have placed another mat with olive paste on the press</t>
-  </si>
-  <si>
     <t>pressR/loading2</t>
   </si>
   <si>
     <t>pressR/loading3</t>
   </si>
   <si>
-    <t>Keep on! By placing another mat Press No2 will be automatically fully loaded</t>
-  </si>
-  <si>
     <t>i//Each press would need to be loaded with at least 20 mats before starting up</t>
   </si>
   <si>
     <t>pressR/loaded</t>
   </si>
   <si>
-    <t>i//This was a laborious manual task but necessary during the cold olive press process</t>
-  </si>
-  <si>
-    <t>i//Good job! You have fully loaded Press No2 and are ready to start pressing</t>
-  </si>
-  <si>
-    <t>You have picked the mat and can now load it on one of the presses</t>
-  </si>
-  <si>
     <t>resetting_millR</t>
   </si>
   <si>
@@ -1121,9 +1088,6 @@
     <t>Good, you are emptying the paste in the mill's tank</t>
   </si>
   <si>
-    <t>i//Good, you're ready to start loading the mats on the presses</t>
-  </si>
-  <si>
     <t>millR/reset</t>
   </si>
   <si>
@@ -1172,29 +1136,296 @@
     <t>You have loaded the can with the olive paste and are ready to lay it on the mat</t>
   </si>
   <si>
-    <t>mat_as_tool</t>
-  </si>
-  <si>
     <t>You need to load the existing mat on the press before using a new mat</t>
   </si>
   <si>
-    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/paste-ready; loader/ready; pressR/empty</t>
-  </si>
-  <si>
     <t>mat_tray</t>
   </si>
   <si>
     <t>Keep on! By placing another mat, Press No2 will be automatically fully loaded</t>
   </si>
   <si>
-    <t>loading_pressR</t>
+    <t>filling_mat</t>
+  </si>
+  <si>
+    <t>loading_pressR; error0_pressR; dropping_mat</t>
+  </si>
+  <si>
+    <t>You have fully loaded the press with mats full of olive paste</t>
+  </si>
+  <si>
+    <t>This was a laborious manual task but necessary during the cold olive press process</t>
+  </si>
+  <si>
+    <t>i//Good, you're ready to start filling the mats with olive paste</t>
+  </si>
+  <si>
+    <t>You have picked the mat and can now load it on one of the presses; i//Keep on filling more mats with olive paste</t>
+  </si>
+  <si>
+    <t>loading_pressR; dropping_mat</t>
+  </si>
+  <si>
+    <t>pressure-good</t>
+  </si>
+  <si>
+    <t>pressing_pressR</t>
+  </si>
+  <si>
+    <t>pressR/pressing</t>
+  </si>
+  <si>
+    <t>pressure-high</t>
+  </si>
+  <si>
+    <t>a/pressR/Press No2 has finished oil extraction and needs to be released</t>
+  </si>
+  <si>
+    <t>pressure-max</t>
+  </si>
+  <si>
+    <t>press-start</t>
+  </si>
+  <si>
+    <t>press-finish</t>
+  </si>
+  <si>
+    <t>pumpR/working</t>
+  </si>
+  <si>
+    <t>pumpR/idle</t>
+  </si>
+  <si>
+    <t>pumpR/ready</t>
+  </si>
+  <si>
+    <t>hand_guide</t>
+  </si>
+  <si>
+    <t>pumpR/crazy</t>
+  </si>
+  <si>
+    <t>hand_bypass</t>
+  </si>
+  <si>
+    <t>No need to stop operating the pump</t>
+  </si>
+  <si>
+    <t>The pump is not working yet, so there is no reason to start pumping water</t>
+  </si>
+  <si>
+    <t>pumpR/motion</t>
+  </si>
+  <si>
+    <t>set the pump to 'ready' state when the press is loaded</t>
+  </si>
+  <si>
+    <t>Good, you have started up the pump using the belt changing bracket</t>
+  </si>
+  <si>
+    <t>i//Pump No2 is set in operation but does not pump water yet</t>
+  </si>
+  <si>
+    <t>Good, you opened the valve that provides water to Press No2</t>
+  </si>
+  <si>
+    <t>pumpR/pressure</t>
+  </si>
+  <si>
+    <t>The pump is giving power to the press so you should not stop it now</t>
+  </si>
+  <si>
+    <t>You should not stop the pumping process while the press is still pressing</t>
+  </si>
+  <si>
+    <t>finishing_pressR</t>
+  </si>
+  <si>
+    <t>changing_wheelR</t>
+  </si>
+  <si>
+    <t>You should not stop the pump while it is still pumping water</t>
+  </si>
+  <si>
+    <t>Good, you have stopped pumping water to the press</t>
+  </si>
+  <si>
+    <t>i//Press No2 is released and the mats are unloaded</t>
+  </si>
+  <si>
+    <t>pressR/releasing</t>
+  </si>
+  <si>
+    <t>boiler_pressure_4500psi; starting_timer; error0_boiler</t>
+  </si>
+  <si>
+    <t>error1_boiler; boiler_pressure_3000psi</t>
+  </si>
+  <si>
+    <t>boiler_pressure_1500psi; dying_away_fire</t>
+  </si>
+  <si>
+    <t>stopping_timer; boiler_pressure_0psi; exhausting_fire</t>
+  </si>
+  <si>
+    <t>stopping_timer; boiler_pressure_4500psi; renewing_fire</t>
+  </si>
+  <si>
+    <t>pumpR_pressure_1500psi; timerP1_goodR</t>
+  </si>
+  <si>
+    <t>pressure-safe</t>
+  </si>
+  <si>
+    <t>pressure-done</t>
+  </si>
+  <si>
+    <t>lifting_barR; timerP1_doneR</t>
+  </si>
+  <si>
+    <t>i//Great! The pressing process for Press No2 has just started!</t>
+  </si>
+  <si>
+    <t>a/pumpR/Supply to Press No2 has very high pressure and there is danger for malfunction</t>
+  </si>
+  <si>
+    <t>i//Good job! Press No2 is now loaded and ready to start pressing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>starting_pressR;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pumpR_pressure_4000psi; timerP1_safeR</t>
+    </r>
+  </si>
+  <si>
+    <t>No need to start operating the pump before loading the corresponding press</t>
+  </si>
+  <si>
+    <t>You need to set the pump in motion first before you start pumping water to the press</t>
+  </si>
+  <si>
+    <t>pumpR/ready:pumpR/crazy</t>
+  </si>
+  <si>
+    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/paste-ready; loader/ready; pressR/loading3; pumpR/crazy</t>
+  </si>
+  <si>
+    <t>opening_bypassR</t>
+  </si>
+  <si>
+    <t>blue events are received from the pump</t>
+  </si>
+  <si>
+    <t>a/pumpR/The water pumped to press No2 exceeded the allowable pressure limits</t>
+  </si>
+  <si>
+    <t>error0_pressR; releasing_pressR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">closing_bypassR; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resetting_pressR</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; dropping_barR; error0_pumpR; timerP0_highR; timerP0_maxR; pumpR_pressure_0psi</t>
+    </r>
+  </si>
+  <si>
+    <t>press-reset</t>
+  </si>
+  <si>
+    <t>millR/waste</t>
+  </si>
+  <si>
+    <t>error0_millR</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resetting_pressR;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dropping_barR; pumpR_pressure_0psi</t>
+    </r>
+  </si>
+  <si>
+    <t>timerP1_highR</t>
+  </si>
+  <si>
+    <t>pumpR_pressure_4500psi; timerP1_maxR; error1_pumpR</t>
+  </si>
+  <si>
+    <t>blue actions are sent to the press with a delay (1')</t>
+  </si>
+  <si>
+    <t>pumpR/boom</t>
+  </si>
+  <si>
+    <t>error0_pumpR</t>
+  </si>
+  <si>
+    <t>damaging_pumpR</t>
+  </si>
+  <si>
+    <t>YOU DAMAGED THE PUMP, YOU MORON!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1301,20 +1532,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1360,9 +1577,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1394,7 +1657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1411,12 +1674,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1437,8 +1709,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1446,14 +1716,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1461,16 +1726,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="20" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="20" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2365,7 +2650,7 @@
   <cols>
     <col min="1" max="1" width="20.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="29" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -2373,370 +2658,370 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>174</v>
+        <v>176</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>169</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>175</v>
+        <v>168</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="37">
+        <v>178</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="30">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>177</v>
+        <v>171</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>172</v>
       </c>
       <c r="D3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" s="37">
+        <v>213</v>
+      </c>
+      <c r="F3" s="30">
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C4" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" t="s">
         <v>178</v>
-      </c>
-      <c r="D4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>192</v>
+        <v>171</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F5" s="37">
+        <v>213</v>
+      </c>
+      <c r="F5" s="30">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="36" t="s">
-        <v>204</v>
+        <v>171</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>199</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>187</v>
+      <c r="B7" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="42">
+        <v>178</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="35">
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>190</v>
+      <c r="B8" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>185</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>191</v>
+      <c r="B9" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="D10" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>202</v>
-      </c>
-      <c r="E10" t="s">
-        <v>186</v>
-      </c>
-      <c r="F10" s="37">
-        <v>0.10416666666666667</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="F11" s="37"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>201</v>
-      </c>
       <c r="E12" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="F12" s="30">
+        <v>7.9861111111111105E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" t="s">
         <v>218</v>
       </c>
-      <c r="F12" s="37">
-        <v>7.9861111111111105E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="C13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>201</v>
+      <c r="D13" s="33" t="s">
+        <v>196</v>
       </c>
       <c r="E13" t="s">
-        <v>218</v>
-      </c>
-      <c r="F13" s="37">
+        <v>213</v>
+      </c>
+      <c r="F13" s="30">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="38" t="s">
-        <v>194</v>
+      <c r="B14" s="31" t="s">
+        <v>189</v>
       </c>
       <c r="C14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="38" t="s">
-        <v>195</v>
+      <c r="B15" s="31" t="s">
+        <v>190</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>202</v>
+        <v>219</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>197</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
-      </c>
-      <c r="F15" s="37">
+        <v>175</v>
+      </c>
+      <c r="F15" s="30">
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>213</v>
+      </c>
+      <c r="F16" s="30">
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="B16" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="F16" s="37">
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="C17" s="36" t="s">
+      <c r="F17" s="30">
+        <v>7.9861111111111105E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>189</v>
-      </c>
-      <c r="F17" s="37">
-        <v>7.9861111111111105E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>226</v>
+      <c r="C18" s="31" t="s">
+        <v>221</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" t="s">
-        <v>218</v>
-      </c>
-      <c r="F18" s="37">
+        <v>213</v>
+      </c>
+      <c r="F18" s="30">
         <v>6.5972222222222224E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
-      </c>
-      <c r="C21" s="36" t="s">
-        <v>210</v>
+        <v>203</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>205</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E21" t="s">
-        <v>180</v>
-      </c>
-      <c r="F21" s="37">
+        <v>175</v>
+      </c>
+      <c r="F21" s="30">
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>230</v>
+        <v>203</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>225</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>231</v>
+        <v>204</v>
+      </c>
+      <c r="E22" s="34" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>208</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>211</v>
+        <v>203</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>206</v>
       </c>
       <c r="D23" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>202</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>216</v>
+      <c r="C24" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>211</v>
       </c>
       <c r="E24" t="s">
-        <v>180</v>
-      </c>
-      <c r="F24" s="37">
+        <v>175</v>
+      </c>
+      <c r="F24" s="30">
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" t="s">
         <v>227</v>
-      </c>
-      <c r="B25" t="s">
-        <v>228</v>
-      </c>
-      <c r="C25" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="D25" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2752,18 +3037,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="16.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17" style="2" customWidth="1"/>
-    <col min="5" max="5" width="41.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="68.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
@@ -2779,1484 +3064,2025 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>279</v>
+      <c r="D2" s="39"/>
+      <c r="E2" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>133</v>
+      <c r="A3" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="44" t="s">
-        <v>122</v>
+        <v>129</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>120</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>123</v>
+      </c>
       <c r="F3" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="20" t="s">
+    <row r="4" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="20" t="s">
-        <v>162</v>
+      <c r="F4" s="18" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>134</v>
+      <c r="A5" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+        <v>129</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>120</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>134</v>
+      <c r="A6" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>150</v>
+        <v>129</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>146</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>280</v>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>135</v>
+      <c r="A8" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>120</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>135</v>
+      <c r="A9" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="3"/>
       <c r="F9" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="50"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="20" t="s">
+      <c r="B17" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="28"/>
-      <c r="F16" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="25"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>138</v>
+      <c r="A18" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="F18" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="25"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
-        <v>156</v>
+      <c r="A20" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="26" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="24" t="s">
+      <c r="F20" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="25"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>148</v>
+      <c r="A22" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="F22" s="26" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="24" t="s">
+      <c r="F22" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="25" t="s">
-        <v>123</v>
+      <c r="D23" s="20"/>
+      <c r="E23" s="23" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
-        <v>139</v>
+      <c r="A24" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="24" t="s">
+    <row r="25" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="25"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>152</v>
+      <c r="A26" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="F26" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>168</v>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="3"/>
       <c r="F28" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="26" t="s">
+    <row r="29" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="48" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="F29" s="26" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="49" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="24" t="s">
+    <row r="30" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="25"/>
-    </row>
-    <row r="31" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="24" t="s">
+      <c r="D30" s="20"/>
+      <c r="E30" s="23"/>
+    </row>
+    <row r="31" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>169</v>
+      <c r="D31" s="20"/>
+      <c r="E31" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
-        <v>141</v>
+      <c r="A32" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="44" t="s">
-        <v>275</v>
+        <v>129</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>270</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="2" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F34" s="2" t="s">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="24" t="s">
+    <row r="37" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="24" t="s">
+      <c r="D37" s="46"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="22" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C39" s="24" t="s">
+      <c r="D38" s="20"/>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E39" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>293</v>
+      <c r="D39" s="20"/>
+      <c r="E39" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="24" t="s">
-        <v>238</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C41" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="25"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E42" s="4"/>
+        <v>230</v>
+      </c>
       <c r="G42" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C43" s="24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E43" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>281</v>
+      <c r="D43" s="20"/>
+      <c r="E43" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="G43" s="22" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="D45" s="3"/>
+        <v>243</v>
+      </c>
       <c r="F45" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" s="24" t="s">
         <v>235</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="E48" s="43"/>
-      <c r="F48" s="26" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D48" s="25"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="24" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="D49" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E49" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="F49" s="26" t="s">
-        <v>263</v>
+        <v>129</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="E49" s="36"/>
+      <c r="F49" s="43" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D52" s="25"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="24" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="F51" s="24" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="26" t="s">
-        <v>249</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D55" s="25"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="24" t="s">
         <v>249</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="24" t="s">
-        <v>246</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="26" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="E56" s="43"/>
-      <c r="F56" s="26" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="26" t="s">
-        <v>246</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="D57" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E57" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="F57" s="26" t="s">
-        <v>291</v>
+    </row>
+    <row r="56" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" s="25"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="24" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="E57" s="36"/>
+      <c r="F57" s="43" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="24" t="s">
-        <v>271</v>
-      </c>
-      <c r="B59" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C59" s="24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C59" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E59" s="25" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="B60" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="F60" s="26" t="s">
-        <v>258</v>
+      <c r="D59" s="20"/>
+      <c r="E59" s="23" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="D60" s="25"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="24" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="B62" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="F62" s="24" t="s">
-        <v>292</v>
+      <c r="D62" s="20"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="22" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="E64" s="4"/>
-    </row>
-    <row r="65" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="24" t="s">
-        <v>323</v>
-      </c>
-      <c r="B65" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="24" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="22" t="s">
+        <v>390</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="22"/>
-      <c r="E65" s="25" t="s">
+      <c r="D65" s="20"/>
+      <c r="E65" s="23" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="49" t="s">
+        <v>311</v>
+      </c>
+      <c r="B68" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="52" t="s">
+        <v>267</v>
+      </c>
+      <c r="D68" s="50" t="s">
+        <v>229</v>
+      </c>
+      <c r="E68" s="51" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D69" s="20"/>
+      <c r="E69" s="23"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="D72" s="25"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="22" t="s">
+        <v>290</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C75" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" s="20"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="22" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="D76" s="25"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="24" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C78" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D78" s="25"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="24" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E79" s="4" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="B66" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D66" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="24" t="s">
-        <v>285</v>
-      </c>
-      <c r="B67" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="B69" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C69" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E69" s="25"/>
-      <c r="F69" s="24" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C70" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="F70" s="26" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="D72" s="3"/>
-      <c r="E72" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="B73" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C73" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D73" s="22"/>
-      <c r="F73" s="24" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B74" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C74" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="D74" s="28"/>
-      <c r="F74" s="26" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B75" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C75" s="26" t="s">
-        <v>286</v>
-      </c>
-      <c r="D75" s="28"/>
-      <c r="F75" s="26" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="26" t="s">
-        <v>295</v>
-      </c>
-      <c r="B76" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C76" s="26" t="s">
-        <v>330</v>
-      </c>
-      <c r="D76" s="28"/>
-      <c r="F76" s="26" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D78" s="45" t="s">
-        <v>329</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="24" t="s">
-        <v>329</v>
-      </c>
-      <c r="B79" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C79" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E79" s="25" t="s">
-        <v>339</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>303</v>
+      <c r="F79" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="20"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="22" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="52" t="s">
+        <v>317</v>
+      </c>
+      <c r="B83" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C83" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="D83" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="E83" s="54" t="s">
+        <v>298</v>
+      </c>
+      <c r="F83" s="55" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="22" t="s">
+        <v>300</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D84" s="20"/>
+      <c r="E84" s="23"/>
+    </row>
+    <row r="85" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="F85" s="22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D87" s="20"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="22" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C89" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D89" s="20"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="22"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="E80" s="4"/>
-      <c r="F80" s="2" t="s">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B91" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C91" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="22"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="B93" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D93" s="20"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C94" s="40" t="s">
+        <v>343</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="G94" s="40" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B95" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D95" s="20"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="22" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C96" s="58" t="s">
+        <v>344</v>
+      </c>
+      <c r="D96" s="25"/>
+      <c r="E96" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="F96" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="G96" s="24"/>
+    </row>
+    <row r="97" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C97" s="58" t="s">
+        <v>389</v>
+      </c>
+      <c r="D97" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="E97" s="36"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+    </row>
+    <row r="98" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="22" t="s">
+        <v>366</v>
+      </c>
+      <c r="B98" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C98" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="F98" s="22" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="49" t="s">
+        <v>366</v>
+      </c>
+      <c r="B99" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="C99" s="49" t="s">
+        <v>267</v>
+      </c>
+      <c r="D99" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="E99" s="51"/>
+      <c r="F99" s="49"/>
+    </row>
+    <row r="100" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C100" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D100" s="20"/>
+      <c r="E100" s="23"/>
+    </row>
+    <row r="101" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="B101" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C101" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D101" s="20"/>
+      <c r="E101" s="23"/>
+    </row>
+    <row r="102" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D102" s="25"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="G102" s="24"/>
+    </row>
+    <row r="103" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C103" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D103" s="25"/>
+      <c r="E103" s="36"/>
+      <c r="F103" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="G103" s="24"/>
+    </row>
+    <row r="104" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="B104" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C104" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D104" s="20"/>
+      <c r="E104" s="23"/>
+    </row>
+    <row r="105" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C105" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D105" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="E105" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="F105" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="G105" s="24"/>
+    </row>
+    <row r="106" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C106" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D106" s="25"/>
+      <c r="E106" s="36"/>
+      <c r="F106" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G106" s="24"/>
+    </row>
+    <row r="107" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B107" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C107" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D107" s="20"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="22" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D108" s="25"/>
+      <c r="E108" s="36"/>
+      <c r="F108" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="G108" s="24"/>
+    </row>
+    <row r="109" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C109" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D109" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="E109" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>357</v>
+      </c>
+      <c r="G109" s="24"/>
+    </row>
+    <row r="110" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="B110" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C110" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D110" s="20"/>
+      <c r="E110" s="23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C111" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D111" s="25"/>
+      <c r="E111" s="36"/>
+      <c r="F111" s="24" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D112" s="25"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="24" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C113" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="D113" s="25"/>
+      <c r="E113" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="G113" s="58" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="D114" s="25"/>
+      <c r="E114" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+    </row>
+    <row r="115" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D115" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="E115" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24"/>
+    </row>
+    <row r="116" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="B116" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C116" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D116" s="20"/>
+      <c r="E116" s="23" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C117" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="D117" s="25"/>
+      <c r="E117" s="36"/>
+      <c r="F117" s="24" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C118" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D118" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="E118" s="36" t="s">
+        <v>388</v>
+      </c>
+      <c r="F118" s="24" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="B82" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C82" s="24" t="s">
+      <c r="E119" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="F120" s="42" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="B121" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E82" s="25"/>
-    </row>
-    <row r="83" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="24" t="s">
-        <v>305</v>
-      </c>
-      <c r="B83" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E83" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="B85" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E85" s="25"/>
-      <c r="F85" s="24" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="B87" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C87" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="24" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="24" t="s">
-        <v>312</v>
-      </c>
-      <c r="B89" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C89" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" s="24"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="24"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="B91" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C91" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="F91" s="24" t="s">
-        <v>317</v>
+      <c r="D121" s="20"/>
+      <c r="E121" s="23" t="s">
+        <v>398</v>
+      </c>
+      <c r="F121" s="22" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -4267,7 +5093,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -4288,90 +5114,104 @@
         <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>341</v>
+    </row>
+    <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>326</v>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Xbox support; process working until pressing; machines work once
- Added Xbox support (Logitech still supported)
- Factory works for all machines besides oil pump and laval
- Added all missing objects to toolbox
- Selection has an empty space after all tools have circulated
- Updates laval reduced model
- Added axis support to factory
- Corrected double-faced material on roof (not supported by OSG)
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="16275" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="240" windowWidth="16275" windowHeight="9600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="422">
   <si>
     <t>Current State</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>a/The engine stopped working due to inadequate steam pressure!</t>
-  </si>
-  <si>
     <t>entry</t>
   </si>
   <si>
@@ -356,36 +353,15 @@
     <t>error1_boiler</t>
   </si>
   <si>
-    <t>belt_powerWheel</t>
-  </si>
-  <si>
     <t>Good job! These belts are used to provide motion from the engine to the machinery</t>
   </si>
   <si>
     <t>belt_wheel</t>
   </si>
   <si>
-    <t>You need someone else to loosen the Laval's power wheel and stretch the belt</t>
-  </si>
-  <si>
-    <t>wrench_powerWheel</t>
-  </si>
-  <si>
-    <t>You need someone else to place and stretch the belt on the driving wheel side</t>
-  </si>
-  <si>
-    <t>You should place the belt on the side of the driving wheel first</t>
-  </si>
-  <si>
     <t>wrench_wheel</t>
   </si>
   <si>
-    <t>You can't loosen the driving wheel</t>
-  </si>
-  <si>
-    <t>detaching_laval_belt; error1_lavalL</t>
-  </si>
-  <si>
     <t>Engine/on</t>
   </si>
   <si>
@@ -395,9 +371,6 @@
     <t>hand_coal</t>
   </si>
   <si>
-    <t>stopping_engine</t>
-  </si>
-  <si>
     <t>Boiler/empty</t>
   </si>
   <si>
@@ -416,9 +389,6 @@
     <t>Matches is one of the ways to light the coals and start the fire</t>
   </si>
   <si>
-    <t>starting_engine</t>
-  </si>
-  <si>
     <t>MachineState</t>
   </si>
   <si>
@@ -446,12 +416,6 @@
     <t>engine/on</t>
   </si>
   <si>
-    <t>lavalL/belt-off</t>
-  </si>
-  <si>
-    <t>lavalL/belt-on</t>
-  </si>
-  <si>
     <t>FactoryState</t>
   </si>
   <si>
@@ -461,54 +425,27 @@
     <t>factory/start</t>
   </si>
   <si>
-    <t>lavalL/idle</t>
-  </si>
-  <si>
     <t>engine/steam</t>
   </si>
   <si>
     <t>a:b#c:d -&gt; go to a if b, or go to c if d</t>
   </si>
   <si>
-    <t>hand_coalfurnace</t>
-  </si>
-  <si>
     <t>engine/ready</t>
   </si>
   <si>
     <t>engine/steam:engine/idle#engine/ready:engine/belt</t>
   </si>
   <si>
-    <t>if engine idle-&gt;engine has steam; if lavalL has belt-&gt;engine ready</t>
-  </si>
-  <si>
-    <t>There is one more component missing from the factory</t>
-  </si>
-  <si>
     <t>engine/belt</t>
   </si>
   <si>
-    <t>LavalL/belt-on</t>
-  </si>
-  <si>
     <t>engine/belt:engine/idle#engine/ready:engine/steam</t>
   </si>
   <si>
-    <t>attaching_belt*; error0_lavalL</t>
-  </si>
-  <si>
-    <t>boiler/idle:boiler/empty; engine/belt:lavalL/belt-on</t>
-  </si>
-  <si>
-    <t>a/boiler/The olive press does not have power!</t>
-  </si>
-  <si>
     <t>i//Great! The boiler's furnace is being loaded with coal</t>
   </si>
   <si>
-    <t>i//Good! You have started up the fire in the boiler's furnace</t>
-  </si>
-  <si>
     <t>a/boiler/Beware! Boiler pressure is marginally low (3,000 psi) for normal operation</t>
   </si>
   <si>
@@ -522,12 +459,6 @@
   </si>
   <si>
     <t>i//Good! You started steam supply to the engine and the whole factory!</t>
-  </si>
-  <si>
-    <t>a/lavalL/A belt is missing from one of the machines</t>
-  </si>
-  <si>
-    <t>i//Great! The Laval separator is ready to be set in motion</t>
   </si>
   <si>
     <t>engine/no-steam:engine/on#engine/belt:engine/ready#engine/idle:engine/steam; boiler/idle:engine/idle#boiler/idle:engine/belt</t>
@@ -851,9 +782,6 @@
     <t>error1_millR</t>
   </si>
   <si>
-    <t>loading_mill1R*; error0_millR</t>
-  </si>
-  <si>
     <t>millR/loading</t>
   </si>
   <si>
@@ -893,9 +821,6 @@
     <t>There is no need to put water in the paste, yet</t>
   </si>
   <si>
-    <t>You are pooring water in the paste to prevent it from becoming too thick</t>
-  </si>
-  <si>
     <t>hand_hatch</t>
   </si>
   <si>
@@ -908,9 +833,6 @@
     <t>i//Good job! The olive paste should be diluted quite often with water</t>
   </si>
   <si>
-    <t>The paste is liquid enough, no need for extra water</t>
-  </si>
-  <si>
     <t>hand_tank</t>
   </si>
   <si>
@@ -962,12 +884,6 @@
     <t>millR/tank-full</t>
   </si>
   <si>
-    <t>Good! You are moving the paste to the loading table</t>
-  </si>
-  <si>
-    <t>hand_wheel, hand_wheel</t>
-  </si>
-  <si>
     <t>hand_sack1R, hand_sack1R</t>
   </si>
   <si>
@@ -992,9 +908,6 @@
     <t>1R = the first sack of the right mill</t>
   </si>
   <si>
-    <t>Good teamwork! You have emptied a whole sack of olives (100 lb) into the right mill</t>
-  </si>
-  <si>
     <t>loader/idle</t>
   </si>
   <si>
@@ -1067,12 +980,6 @@
     <t>pressR/loading</t>
   </si>
   <si>
-    <t>pressR/loading2</t>
-  </si>
-  <si>
-    <t>pressR/loading3</t>
-  </si>
-  <si>
     <t>i//Each press would need to be loaded with at least 20 mats before starting up</t>
   </si>
   <si>
@@ -1115,9 +1022,6 @@
     <t>scooping_pulp</t>
   </si>
   <si>
-    <t>You don't have any olive paste in the tank to load the mat</t>
-  </si>
-  <si>
     <t>get-pulp</t>
   </si>
   <si>
@@ -1142,12 +1046,6 @@
     <t>mat_tray</t>
   </si>
   <si>
-    <t>Keep on! By placing another mat, Press No2 will be automatically fully loaded</t>
-  </si>
-  <si>
-    <t>filling_mat</t>
-  </si>
-  <si>
     <t>loading_pressR; error0_pressR; dropping_mat</t>
   </si>
   <si>
@@ -1196,9 +1094,6 @@
     <t>pumpR/idle</t>
   </si>
   <si>
-    <t>pumpR/ready</t>
-  </si>
-  <si>
     <t>hand_guide</t>
   </si>
   <si>
@@ -1220,12 +1115,6 @@
     <t>set the pump to 'ready' state when the press is loaded</t>
   </si>
   <si>
-    <t>Good, you have started up the pump using the belt changing bracket</t>
-  </si>
-  <si>
-    <t>i//Pump No2 is set in operation but does not pump water yet</t>
-  </si>
-  <si>
     <t>Good, you opened the valve that provides water to Press No2</t>
   </si>
   <si>
@@ -1241,9 +1130,6 @@
     <t>finishing_pressR</t>
   </si>
   <si>
-    <t>changing_wheelR</t>
-  </si>
-  <si>
     <t>You should not stop the pump while it is still pumping water</t>
   </si>
   <si>
@@ -1269,9 +1155,6 @@
   </si>
   <si>
     <t>stopping_timer; boiler_pressure_4500psi; renewing_fire</t>
-  </si>
-  <si>
-    <t>pumpR_pressure_1500psi; timerP1_goodR</t>
   </si>
   <si>
     <t>pressure-safe</t>
@@ -1320,12 +1203,6 @@
   </si>
   <si>
     <t>You need to set the pump in motion first before you start pumping water to the press</t>
-  </si>
-  <si>
-    <t>pumpR/ready:pumpR/crazy</t>
-  </si>
-  <si>
-    <t>boiler/idle; engine/idle; lavalL/belt-off; millR/paste-ready; loader/ready; pressR/loading3; pumpR/crazy</t>
   </si>
   <si>
     <t>opening_bypassR</t>
@@ -1376,30 +1253,6 @@
     <t>error0_millR</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="4" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>resetting_pressR;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dropping_barR; pumpR_pressure_0psi</t>
-    </r>
-  </si>
-  <si>
     <t>timerP1_highR</t>
   </si>
   <si>
@@ -1412,20 +1265,212 @@
     <t>pumpR/boom</t>
   </si>
   <si>
-    <t>error0_pumpR</t>
-  </si>
-  <si>
     <t>damaging_pumpR</t>
   </si>
   <si>
-    <t>YOU DAMAGED THE PUMP, YOU MORON!</t>
+    <t>dropping_barR; pumpR_pressure_0psi</t>
+  </si>
+  <si>
+    <t>resetting_pressR; error0_pumpR</t>
+  </si>
+  <si>
+    <t>pumpR/crazy-ready</t>
+  </si>
+  <si>
+    <t>pumpR/motion-ready</t>
+  </si>
+  <si>
+    <t>Press No2 is still empty, you need to load it before starting the pressing process</t>
+  </si>
+  <si>
+    <t>stopping_pumpR</t>
+  </si>
+  <si>
+    <t>You have stopped the operation of the pump by rolling the belt back to the "crazy" wheel</t>
+  </si>
+  <si>
+    <t>pumpR/crazy-ready:pumpR/crazy#pumpR/motion-ready:pumpR/motion</t>
+  </si>
+  <si>
+    <t>pumpR/motion-ready:pressR/loaded</t>
+  </si>
+  <si>
+    <t>set pump to 'ready in motion' if the press is loaded (after bracket change)</t>
+  </si>
+  <si>
+    <t>removing_matsR</t>
+  </si>
+  <si>
+    <t>fillingup_pressR</t>
+  </si>
+  <si>
+    <t>press-fillup</t>
+  </si>
+  <si>
+    <t>hand_sack1R</t>
+  </si>
+  <si>
+    <t>The sack is too heavy (approx. 350 lb) to lift by yourself</t>
+  </si>
+  <si>
+    <t>You are pouring water in the paste to prevent it from becoming too thick</t>
+  </si>
+  <si>
+    <t>The paste is liquid enough, no need to add extra water</t>
+  </si>
+  <si>
+    <t>Good! You are moving the paste to the loading table and emptying it in the large tank</t>
+  </si>
+  <si>
+    <t>hand_sack2R, hand_sack2R</t>
+  </si>
+  <si>
+    <t>The olives are not completeley crashed yet, wait a little longer until they become a smooth paste</t>
+  </si>
+  <si>
+    <t>loading_mill1R*</t>
+  </si>
+  <si>
+    <t>loading_mill2R*</t>
+  </si>
+  <si>
+    <t>You need to spread the paste on the mat before you pick it up</t>
+  </si>
+  <si>
+    <t>You need someone else to spread the paste on the straw mat with his hands</t>
+  </si>
+  <si>
+    <t>canful_mat, hand_mat</t>
+  </si>
+  <si>
+    <t>filling_mat*</t>
+  </si>
+  <si>
+    <t>detaching_laval_belt; error1_lavalR</t>
+  </si>
+  <si>
+    <t>attaching_belt*; error0_lavalR</t>
+  </si>
+  <si>
+    <t>LavalR/belt-on</t>
+  </si>
+  <si>
+    <t>lavalR/belt-on</t>
+  </si>
+  <si>
+    <t>lavalR/belt-off</t>
+  </si>
+  <si>
+    <t>lavalR/idle</t>
+  </si>
+  <si>
+    <t>wrench_crazyW</t>
+  </si>
+  <si>
+    <t>belt_crazyW</t>
+  </si>
+  <si>
+    <t>boiler/idle:boiler/empty; engine/belt:lavalR/belt-on</t>
+  </si>
+  <si>
+    <t>if engine idle-&gt;engine has steam; if lavalR has belt-&gt;engine ready</t>
+  </si>
+  <si>
+    <t>a/lavalR/A belt is missing from one of the machines</t>
+  </si>
+  <si>
+    <t>You need someone else to loosen the Laval's "crazy" wheel while stretching the belt</t>
+  </si>
+  <si>
+    <t>You need someone else to place and stretch the belt on the power wheel side</t>
+  </si>
+  <si>
+    <t>You should place the belt on the side of the power wheel first</t>
+  </si>
+  <si>
+    <t>You can't loosen the power wheel, but try with the Laval's "crazy" wheel</t>
+  </si>
+  <si>
+    <t>i//Great! The Laval separator No2 is ready to be set in motion</t>
+  </si>
+  <si>
+    <t>a/boiler/The boiler is not working, you need to start it up!</t>
+  </si>
+  <si>
+    <t>i//Good! The boiler is now burning and producing steam!</t>
+  </si>
+  <si>
+    <t>The boiler has enough pressure, no need for more coal</t>
+  </si>
+  <si>
+    <t>a/engine/The engine stopped working due to inadequate steam pressure!</t>
+  </si>
+  <si>
+    <t>You cannot turn on the engine before you fix all components of the factory</t>
+  </si>
+  <si>
+    <t>a/engine/The steam supply to the engine is turned off</t>
+  </si>
+  <si>
+    <t>error1_engine</t>
+  </si>
+  <si>
+    <t>starting_engine; error0_engine</t>
+  </si>
+  <si>
+    <t>stopping_engine; error1_engine</t>
+  </si>
+  <si>
+    <t>a/engine/There is not enough steam to keep the engine working</t>
+  </si>
+  <si>
+    <t>millR/empty; pumpR/crazy</t>
+  </si>
+  <si>
+    <t>belt_wheel, wrench_crazyW</t>
+  </si>
+  <si>
+    <t>boiler/idle; engine/idle; lavalR/belt-off; millR/empty; loader/idle; pressR/idle; pumpR/idle</t>
+  </si>
+  <si>
+    <t>Good teamwork! You have emptied a whole sack of olives (350 lb) into the right mill</t>
+  </si>
+  <si>
+    <t>You don't have any olive paste in the tank, so you cannot start loading the mats</t>
+  </si>
+  <si>
+    <t>Good, you have set the pump in motion by changing the belt from the "crazy" to the power wheel</t>
+  </si>
+  <si>
+    <t>millR/done</t>
+  </si>
+  <si>
+    <t>pressR/done</t>
+  </si>
+  <si>
+    <t>error1_pumpR</t>
+  </si>
+  <si>
+    <t>a/pumpR/Pump No2 is ready to start pumping water to the corresponding press</t>
+  </si>
+  <si>
+    <t>starting_pumpR; error0_pumpR</t>
+  </si>
+  <si>
+    <t>a/pumpR/Pump No2 is set in operation but does not pump water yet</t>
+  </si>
+  <si>
+    <t>i//Great! Pump No2 is now pumping water to the corresponding press</t>
+  </si>
+  <si>
+    <t>pumpR_pressure_1500psi; timerP1_goodR; error0_pumpR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1625,7 +1670,14 @@
     <font>
       <i/>
       <sz val="10"/>
-      <color theme="4" tint="-0.499984740745262"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1688,7 +1740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1753,9 +1805,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2658,39 +2716,39 @@
   <sheetData>
     <row r="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="C1" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>192</v>
-      </c>
       <c r="F1" s="9" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="F2" s="30">
         <v>7.2916666666666671E-2</v>
@@ -2698,16 +2756,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="E3" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F3" s="30">
         <v>3.125E-2</v>
@@ -2715,27 +2773,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F5" s="30">
         <v>4.1666666666666664E-2</v>
@@ -2743,27 +2801,27 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F7" s="35">
         <v>3.4722222222222224E-2</v>
@@ -2771,41 +2829,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E10" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="F10" s="30">
         <v>0.10416666666666667</v>
@@ -2813,28 +2871,28 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="31" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="F11" s="30"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="31" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F12" s="30">
         <v>7.9861111111111105E-2</v>
@@ -2842,16 +2900,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F13" s="30">
         <v>6.25E-2</v>
@@ -2859,27 +2917,27 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="C14" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="31" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="F15" s="30">
         <v>3.4722222222222224E-2</v>
@@ -2887,19 +2945,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F16" s="30">
         <v>7.2916666666666671E-2</v>
@@ -2907,16 +2965,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="31" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="F17" s="30">
         <v>7.9861111111111105E-2</v>
@@ -2924,14 +2982,14 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F18" s="30">
         <v>6.5972222222222224E-2</v>
@@ -2939,27 +2997,27 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="E21" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="F21" s="30">
         <v>7.9861111111111105E-2</v>
@@ -2967,44 +3025,44 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="34" t="s">
         <v>203</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="D22" t="s">
-        <v>204</v>
-      </c>
-      <c r="E22" s="34" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="E24" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="F24" s="30">
         <v>9.7222222222222224E-2</v>
@@ -3012,16 +3070,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3037,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3074,74 +3132,74 @@
         <v>91</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>156</v>
+        <v>398</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="21" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>95</v>
@@ -3149,68 +3207,68 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="21" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>158</v>
+        <v>399</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>94</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>96</v>
@@ -3218,299 +3276,312 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="21" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="26"/>
       <c r="F15" s="27" t="s">
-        <v>99</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C16" s="49" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D16" s="50"/>
       <c r="E16" s="51"/>
       <c r="F16" s="49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>150</v>
+        <v>402</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="23" t="s">
-        <v>121</v>
+        <v>406</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="20"/>
-      <c r="E25" s="23"/>
+      <c r="E25" s="23" t="s">
+        <v>404</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21" t="s">
-        <v>128</v>
+        <v>405</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
@@ -3521,10 +3592,10 @@
     </row>
     <row r="29" spans="1:7" s="49" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B29" s="48" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C29" s="49" t="s">
         <v>92</v>
@@ -3532,1557 +3603,1741 @@
       <c r="D29" s="50"/>
       <c r="E29" s="51"/>
       <c r="F29" s="49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
-        <v>143</v>
+        <v>387</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="20"/>
       <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="20"/>
       <c r="E31" s="23" t="s">
-        <v>117</v>
+        <v>382</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>164</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>270</v>
+        <v>409</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>152</v>
+        <v>384</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>154</v>
+        <v>383</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>111</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>112</v>
+        <v>388</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>113</v>
+        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>108</v>
+        <v>389</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>114</v>
+        <v>395</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>138</v>
+        <v>386</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>116</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44" t="s">
-        <v>139</v>
+        <v>385</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D37" s="46"/>
       <c r="E37" s="47"/>
       <c r="F37" s="45" t="s">
-        <v>165</v>
+        <v>397</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="20"/>
       <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="23" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>232</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="D40" s="59"/>
+      <c r="E40" s="58"/>
       <c r="F40" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="23"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="G43" s="22" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>277</v>
+        <v>209</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="20"/>
+      <c r="E44" s="23" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C47" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" s="20"/>
-      <c r="E47" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="D48" s="25"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="24" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="43" t="s">
-        <v>258</v>
+        <v>119</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>242</v>
+        <v>207</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="23" t="s">
+        <v>234</v>
+      </c>
+      <c r="F51" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="F51" s="22" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="52" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>129</v>
+      <c r="A52" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="D52" s="25"/>
       <c r="E52" s="36"/>
       <c r="F52" s="24" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>244</v>
+        <v>218</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B54" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="B55" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="24" t="s">
-        <v>249</v>
+        <v>119</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="E53" s="36"/>
+      <c r="F53" s="43" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="E55" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="F55" s="22" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D56" s="25"/>
       <c r="E56" s="36"/>
       <c r="F56" s="24" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="24" t="s">
-        <v>241</v>
-      </c>
-      <c r="B57" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="E57" s="36"/>
-      <c r="F57" s="43" t="s">
-        <v>286</v>
+        <v>372</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>310</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="20"/>
       <c r="E59" s="23" t="s">
-        <v>264</v>
+        <v>235</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="24" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D60" s="25"/>
       <c r="E60" s="36"/>
       <c r="F60" s="24" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="B62" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="23"/>
-      <c r="F62" s="22" t="s">
-        <v>287</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" s="25"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="24" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D62" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="E62" s="36"/>
+      <c r="F62" s="43" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>252</v>
+        <v>222</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>313</v>
+        <v>237</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="B65" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C65" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="23" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="B67" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="23" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="49" t="s">
-        <v>311</v>
-      </c>
-      <c r="B68" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="C68" s="52" t="s">
-        <v>267</v>
-      </c>
-      <c r="D68" s="50" t="s">
-        <v>229</v>
-      </c>
-      <c r="E68" s="51" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="B69" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C69" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="23"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" s="20"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="22" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="D67" s="25"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="D68" s="25"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>280</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
-        <v>291</v>
+        <v>349</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D71" s="20"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="22" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E71" s="23" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>291</v>
+        <v>349</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C72" s="24" t="s">
-        <v>292</v>
-      </c>
-      <c r="D72" s="25"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D73" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="20"/>
+      <c r="E73" s="23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="60" t="s">
+        <v>280</v>
+      </c>
+      <c r="B74" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" s="64" t="s">
+        <v>241</v>
+      </c>
+      <c r="D74" s="61" t="s">
+        <v>414</v>
+      </c>
+      <c r="E74" s="62" t="s">
         <v>290</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C75" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D75" s="20"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="22" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="B76" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D76" s="25"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="24" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C77" s="24" t="s">
-        <v>281</v>
-      </c>
-      <c r="D77" s="25"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="24" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="24" t="s">
-        <v>290</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="D78" s="25"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="24" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:6" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="45" t="s">
+        <v>414</v>
+      </c>
+      <c r="B75" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" s="46"/>
+      <c r="E75" s="47"/>
+    </row>
+    <row r="76" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D76" s="20"/>
+      <c r="E76" s="23"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D78" s="20"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>290</v>
+        <v>262</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>326</v>
+        <v>119</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="D79" s="25"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="24" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E80" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="22" t="s">
-        <v>317</v>
-      </c>
-      <c r="B81" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C81" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="20"/>
-      <c r="E81" s="23"/>
-      <c r="F81" s="22" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C82" s="2" t="s">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="20"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="22" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B83" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="D83" s="25"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D84" s="25"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="24" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="D85" s="25"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="24" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="52" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="52" t="s">
-        <v>317</v>
-      </c>
-      <c r="B83" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="C83" s="52" t="s">
-        <v>281</v>
-      </c>
-      <c r="D83" s="53" t="s">
+      <c r="E87" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E83" s="54" t="s">
-        <v>298</v>
-      </c>
-      <c r="F83" s="55" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="B84" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C84" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D84" s="20"/>
-      <c r="E84" s="23"/>
-    </row>
-    <row r="85" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="22" t="s">
-        <v>299</v>
-      </c>
-      <c r="B85" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C85" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D85" s="20"/>
-      <c r="E85" s="23" t="s">
-        <v>309</v>
-      </c>
-      <c r="F85" s="22" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="22" t="s">
-        <v>303</v>
-      </c>
-      <c r="B87" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C87" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" s="20"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="22" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="22" t="s">
-        <v>304</v>
-      </c>
-      <c r="B89" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C89" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" s="20"/>
-      <c r="E89" s="23"/>
-      <c r="F89" s="22"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="E90" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="22" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="B91" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C91" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D91" s="20"/>
       <c r="E91" s="23"/>
-      <c r="F91" s="22"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F91" s="22" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="E92" s="4" t="s">
-        <v>336</v>
+        <v>260</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="22" t="s">
-        <v>307</v>
-      </c>
-      <c r="B93" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C93" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D93" s="20"/>
-      <c r="E93" s="23"/>
-      <c r="F93" s="22" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C94" s="40" t="s">
-        <v>343</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="G94" s="40" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="52" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="52" t="s">
+        <v>286</v>
+      </c>
+      <c r="B94" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="D94" s="53" t="s">
+        <v>262</v>
+      </c>
+      <c r="E94" s="54" t="s">
+        <v>269</v>
+      </c>
+      <c r="F94" s="55" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="22" t="s">
-        <v>339</v>
+        <v>271</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C95" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D95" s="20"/>
       <c r="E95" s="23"/>
-      <c r="F95" s="22" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="B96" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C96" s="58" t="s">
-        <v>344</v>
-      </c>
-      <c r="D96" s="25"/>
-      <c r="E96" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="F96" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="G96" s="24"/>
-    </row>
-    <row r="97" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="B97" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="C97" s="58" t="s">
-        <v>389</v>
-      </c>
-      <c r="D97" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="E97" s="36"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
+    </row>
+    <row r="96" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C96" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D96" s="20"/>
+      <c r="E96" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="98" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="22" t="s">
-        <v>366</v>
+        <v>274</v>
       </c>
       <c r="B98" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C98" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D98" s="20"/>
-      <c r="E98" s="23" t="s">
-        <v>387</v>
-      </c>
+      <c r="E98" s="23"/>
       <c r="F98" s="22" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="49" t="s">
-        <v>366</v>
-      </c>
-      <c r="B99" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="C99" s="49" t="s">
-        <v>267</v>
-      </c>
-      <c r="D99" s="50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E99" s="51"/>
-      <c r="F99" s="49"/>
-    </row>
-    <row r="100" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="22" t="s">
-        <v>346</v>
-      </c>
-      <c r="B100" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C100" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D100" s="20"/>
-      <c r="E100" s="23"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="101" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="22" t="s">
-        <v>349</v>
+        <v>276</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C101" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D101" s="20"/>
       <c r="E101" s="23"/>
-    </row>
-    <row r="102" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F101" s="22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>349</v>
+        <v>276</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C102" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C102" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="G102" s="40" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="20"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B104" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C104" s="57" t="s">
+        <v>310</v>
+      </c>
+      <c r="D104" s="25"/>
+      <c r="E104" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="F104" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="G104" s="24"/>
+    </row>
+    <row r="105" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B105" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="D102" s="25"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="24" t="s">
-        <v>380</v>
-      </c>
-      <c r="G102" s="24"/>
-    </row>
-    <row r="103" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C103" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D103" s="25"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="G103" s="24"/>
-    </row>
-    <row r="104" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="B104" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C104" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D104" s="20"/>
-      <c r="E104" s="23"/>
-    </row>
-    <row r="105" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C105" s="24" t="s">
-        <v>348</v>
-      </c>
       <c r="D105" s="25" t="s">
-        <v>353</v>
-      </c>
-      <c r="E105" s="36" t="s">
-        <v>362</v>
-      </c>
-      <c r="F105" s="24" t="s">
-        <v>355</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="E105" s="36"/>
+      <c r="F105" s="24"/>
       <c r="G105" s="24"/>
     </row>
-    <row r="106" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C106" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D106" s="25"/>
-      <c r="E106" s="36"/>
-      <c r="F106" s="24" t="s">
-        <v>381</v>
-      </c>
-      <c r="G106" s="24"/>
-    </row>
-    <row r="107" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="B107" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C107" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D107" s="20"/>
-      <c r="E107" s="23"/>
-      <c r="F107" s="22" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C108" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="D108" s="25"/>
-      <c r="E108" s="36"/>
-      <c r="F108" s="24" t="s">
-        <v>351</v>
-      </c>
-      <c r="G108" s="24"/>
-    </row>
-    <row r="109" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C109" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D109" s="25" t="s">
-        <v>345</v>
-      </c>
-      <c r="E109" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="F109" s="24" t="s">
-        <v>357</v>
-      </c>
-      <c r="G109" s="24"/>
+    <row r="106" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D106" s="20"/>
+      <c r="E106" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="F106" s="22" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="63" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="B107" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C107" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="D107" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="E107" s="62" t="s">
+        <v>366</v>
+      </c>
+      <c r="F107" s="60"/>
+    </row>
+    <row r="108" spans="1:7" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="45" t="s">
+        <v>415</v>
+      </c>
+      <c r="B108" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D108" s="46"/>
+      <c r="E108" s="47"/>
+    </row>
+    <row r="109" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="B109" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C109" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="23"/>
     </row>
     <row r="110" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="22" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D110" s="20"/>
-      <c r="E110" s="23" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E110" s="23"/>
+    </row>
+    <row r="111" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C111" s="24" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="D111" s="25"/>
       <c r="E111" s="36"/>
       <c r="F111" s="24" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+      <c r="G111" s="24"/>
+    </row>
+    <row r="112" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C112" s="24" t="s">
-        <v>350</v>
+        <v>315</v>
       </c>
       <c r="D112" s="25"/>
       <c r="E112" s="36"/>
       <c r="F112" s="24" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C113" s="24" t="s">
-        <v>337</v>
-      </c>
-      <c r="D113" s="25"/>
-      <c r="E113" s="36" t="s">
-        <v>379</v>
-      </c>
-      <c r="G113" s="58" t="s">
-        <v>395</v>
+        <v>317</v>
+      </c>
+      <c r="G112" s="24"/>
+    </row>
+    <row r="113" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="B113" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C113" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D113" s="20"/>
+      <c r="E113" s="23" t="s">
+        <v>416</v>
+      </c>
+      <c r="F113" s="22" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="114" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="D114" s="25"/>
+        <v>119</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D114" s="25" t="s">
+        <v>318</v>
+      </c>
       <c r="E114" s="36" t="s">
-        <v>375</v>
-      </c>
-      <c r="F114" s="24"/>
+        <v>418</v>
+      </c>
+      <c r="F114" s="24" t="s">
+        <v>413</v>
+      </c>
       <c r="G114" s="24"/>
     </row>
     <row r="115" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D115" s="25" t="s">
-        <v>358</v>
-      </c>
-      <c r="E115" s="57" t="s">
-        <v>361</v>
-      </c>
-      <c r="F115" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="C115" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D115" s="25"/>
+      <c r="E115" s="36"/>
+      <c r="F115" s="24" t="s">
+        <v>342</v>
+      </c>
       <c r="G115" s="24"/>
     </row>
     <row r="116" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="22" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="B116" s="22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C116" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D116" s="20"/>
-      <c r="E116" s="23" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E116" s="23"/>
+    </row>
+    <row r="117" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="D117" s="25"/>
-      <c r="E117" s="36"/>
+        <v>313</v>
+      </c>
+      <c r="D117" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="E117" s="36" t="s">
+        <v>361</v>
+      </c>
       <c r="F117" s="24" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+      <c r="G117" s="24"/>
+    </row>
+    <row r="118" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>358</v>
+        <v>318</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C118" s="24" t="s">
-        <v>350</v>
-      </c>
-      <c r="D118" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="D118" s="25"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="G118" s="24"/>
+    </row>
+    <row r="119" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B119" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C119" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D119" s="20"/>
+      <c r="E119" s="23" t="s">
+        <v>416</v>
+      </c>
+      <c r="F119" s="22" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C120" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D120" s="25"/>
+      <c r="E120" s="36"/>
+      <c r="F120" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="G120" s="24"/>
+    </row>
+    <row r="121" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C121" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D121" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="E121" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="F121" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G121" s="24"/>
+    </row>
+    <row r="122" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="B122" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D122" s="20"/>
+      <c r="E122" s="23" t="s">
+        <v>421</v>
+      </c>
+      <c r="F122" s="22" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C123" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D123" s="25"/>
+      <c r="E123" s="36"/>
+      <c r="F123" s="24" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C124" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D124" s="25"/>
+      <c r="E124" s="36"/>
+      <c r="F124" s="24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="D125" s="25"/>
+      <c r="E125" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="G125" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="E118" s="36" t="s">
-        <v>388</v>
-      </c>
-      <c r="F118" s="24" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="F120" s="42" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="22" t="s">
-        <v>396</v>
-      </c>
-      <c r="B121" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="C121" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D121" s="20"/>
-      <c r="E121" s="23" t="s">
-        <v>398</v>
-      </c>
-      <c r="F121" s="22" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="D122" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E122" s="4" t="s">
-        <v>397</v>
+    </row>
+    <row r="126" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D126" s="25"/>
+      <c r="E126" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="F126" s="24"/>
+      <c r="G126" s="24"/>
+    </row>
+    <row r="127" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D127" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="E127" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="F127" s="24"/>
+      <c r="G127" s="24"/>
+    </row>
+    <row r="128" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="B128" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C128" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D128" s="20"/>
+      <c r="E128" s="23" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D129" s="25"/>
+      <c r="E129" s="36"/>
+      <c r="F129" s="24" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C130" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="D130" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="E130" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="F130" s="24" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F132" s="42" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="B133" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C133" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D133" s="20"/>
+      <c r="E133" s="23" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -5093,9 +5348,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -5114,104 +5369,118 @@
         <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>383</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>149</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>385</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>229</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>307</v>
+        <v>276</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>354</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated version with various fixes
- Saves correctly log file (make exe from trial, not practice)
- Deactivate collision in case player(s) stuck (keypad numbers)
- Smoke shader loads correctly in exe
- Scale indicator updated to kgs and added factor in xlsx (to convert
kg/lb in degrees of angle)
- Added the exe in full screen, with support for the above
</commit_message>
<xml_diff>
--- a/OLiVE_StateMachine.xlsx
+++ b/OLiVE_StateMachine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="16275" windowHeight="9540" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="16275" windowHeight="9540" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3573" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3575" uniqueCount="866">
   <si>
     <t>Current State</t>
   </si>
@@ -2511,9 +2511,6 @@
     <t>weigh-reminder</t>
   </si>
   <si>
-    <t>weighing_pitcher[3, 160]; increasing_total[3,160]; timerS1_reminder[30]</t>
-  </si>
-  <si>
     <t>error2_scale</t>
   </si>
   <si>
@@ -2766,9 +2763,6 @@
     <t>pipe connector</t>
   </si>
   <si>
-    <t>weighing_pitcher[3, 160]; increasing_total[3,160]; error0_scale; timerS0_reminder</t>
-  </si>
-  <si>
     <t>welcome</t>
   </si>
   <si>
@@ -2821,6 +2815,18 @@
   </si>
   <si>
     <t>producing %s lbs of olive oil.</t>
+  </si>
+  <si>
+    <t>weighing_pitcher[3, 160, 6]; increasing_total[3,160]; error0_scale; timerS0_reminder</t>
+  </si>
+  <si>
+    <t>weighing_pitcher[3, 160,6]; increasing_total[3,160]; timerS1_reminder[30]</t>
+  </si>
+  <si>
+    <t>weighing pitcher: last number is factor*10 (to make it int)</t>
+  </si>
+  <si>
+    <t>weighing_pitcher[3, 160, 6]; increasing_total[3,160]; timerS1_reminder[30]</t>
   </si>
 </sst>
 </file>
@@ -4543,10 +4549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G316"/>
+  <dimension ref="A1:H316"/>
   <sheetViews>
     <sheetView topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="E315" sqref="E315"/>
+      <selection activeCell="A314" sqref="A314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4612,12 +4618,12 @@
         <v>100</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="25" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G3" s="23"/>
     </row>
@@ -4678,10 +4684,10 @@
         <v>100</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>791</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5060,7 +5066,7 @@
         <v>108</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F30" s="80" t="s">
         <v>95</v>
@@ -5146,7 +5152,7 @@
         <v>735</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -5163,7 +5169,7 @@
         <v>736</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -5183,7 +5189,7 @@
         <v>587</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -5203,7 +5209,7 @@
         <v>588</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>208</v>
@@ -5315,7 +5321,7 @@
         <v>100</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>696</v>
@@ -5431,7 +5437,7 @@
         <v>100</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>447</v>
@@ -5455,7 +5461,7 @@
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="22" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>756</v>
@@ -5485,7 +5491,7 @@
         <v>100</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D55" s="24"/>
       <c r="E55" s="34"/>
@@ -5563,12 +5569,12 @@
         <v>100</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="34"/>
       <c r="F60" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -5742,18 +5748,18 @@
         <v>453</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>532</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B72" s="21" t="s">
         <v>100</v>
@@ -5764,12 +5770,12 @@
       <c r="D72" s="19"/>
       <c r="E72" s="22"/>
       <c r="F72" s="21" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>100</v>
@@ -5910,7 +5916,7 @@
         <v>738</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -5927,7 +5933,7 @@
         <v>737</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -5947,7 +5953,7 @@
         <v>589</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -5967,7 +5973,7 @@
         <v>590</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>208</v>
@@ -6079,7 +6085,7 @@
         <v>100</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>696</v>
@@ -6195,7 +6201,7 @@
         <v>100</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>194</v>
@@ -6219,7 +6225,7 @@
       </c>
       <c r="D99" s="19"/>
       <c r="E99" s="22" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>756</v>
@@ -6249,7 +6255,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D101" s="24"/>
       <c r="E101" s="34"/>
@@ -6316,7 +6322,7 @@
       <c r="D105" s="24"/>
       <c r="E105" s="34"/>
       <c r="F105" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -6327,12 +6333,12 @@
         <v>100</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D106" s="24"/>
       <c r="E106" s="34"/>
       <c r="F106" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -6506,18 +6512,18 @@
         <v>393</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>531</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="21" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B118" s="21" t="s">
         <v>100</v>
@@ -6528,12 +6534,12 @@
       <c r="D118" s="19"/>
       <c r="E118" s="22"/>
       <c r="F118" s="21" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>100</v>
@@ -6657,7 +6663,7 @@
     </row>
     <row r="127" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="21" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B127" s="21" t="s">
         <v>100</v>
@@ -6667,15 +6673,15 @@
       </c>
       <c r="D127" s="19"/>
       <c r="E127" s="22" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F127" s="21" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B128" s="25" t="s">
         <v>100</v>
@@ -6685,7 +6691,7 @@
       </c>
       <c r="E128" s="85"/>
       <c r="F128" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -6700,10 +6706,10 @@
       </c>
       <c r="D129" s="19"/>
       <c r="E129" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F129" s="21" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -7015,7 +7021,7 @@
         <v>725</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="149" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -7031,7 +7037,7 @@
       <c r="D149" s="19"/>
       <c r="E149" s="22"/>
       <c r="F149" s="21" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -7071,7 +7077,7 @@
         <v>539</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G151" s="68" t="s">
         <v>366</v>
@@ -7417,7 +7423,7 @@
         <v>726</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="172" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -7433,7 +7439,7 @@
       <c r="D172" s="19"/>
       <c r="E172" s="22"/>
       <c r="F172" s="21" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -7473,7 +7479,7 @@
         <v>540</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G174" s="68" t="s">
         <v>366</v>
@@ -7905,7 +7911,7 @@
         <v>413</v>
       </c>
       <c r="E199" s="34" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F199" s="23" t="s">
         <v>608</v>
@@ -7978,7 +7984,7 @@
         <v>419</v>
       </c>
       <c r="E203" s="34" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F203" s="23" t="s">
         <v>648</v>
@@ -8136,7 +8142,7 @@
         <v>418</v>
       </c>
       <c r="E212" s="34" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F212" s="23" t="s">
         <v>649</v>
@@ -8355,7 +8361,7 @@
         <v>241</v>
       </c>
       <c r="E225" s="34" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F225" s="23" t="s">
         <v>608</v>
@@ -8428,7 +8434,7 @@
         <v>239</v>
       </c>
       <c r="E229" s="34" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F229" s="23" t="s">
         <v>648</v>
@@ -8584,7 +8590,7 @@
         <v>243</v>
       </c>
       <c r="E238" s="34" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F238" s="23" t="s">
         <v>649</v>
@@ -9261,7 +9267,7 @@
         <v>369</v>
       </c>
       <c r="E280" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F280" s="2" t="s">
         <v>351</v>
@@ -9366,7 +9372,7 @@
         <v>369</v>
       </c>
       <c r="E286" s="48" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="287" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
@@ -9620,7 +9626,7 @@
         <v>364</v>
       </c>
       <c r="E302" s="4" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F302" s="2" t="s">
         <v>351</v>
@@ -9656,7 +9662,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A305" s="2" t="s">
         <v>364</v>
       </c>
@@ -9673,7 +9679,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306" s="2" t="s">
         <v>364</v>
       </c>
@@ -9693,7 +9699,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="307" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A307" s="21" t="s">
         <v>350</v>
       </c>
@@ -9711,7 +9717,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="308" spans="1:7" s="46" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" s="46" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A308" s="46" t="s">
         <v>350</v>
       </c>
@@ -9728,7 +9734,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="309" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A309" s="21" t="s">
         <v>371</v>
       </c>
@@ -9741,7 +9747,7 @@
       <c r="D309" s="19"/>
       <c r="E309" s="22"/>
     </row>
-    <row r="310" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A310" s="21" t="s">
         <v>764</v>
       </c>
@@ -9759,7 +9765,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
         <v>764</v>
       </c>
@@ -9773,13 +9779,16 @@
         <v>374</v>
       </c>
       <c r="E311" s="4" t="s">
-        <v>768</v>
+        <v>863</v>
       </c>
       <c r="G311" s="70" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="312" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H311" s="2" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A312" s="21" t="s">
         <v>374</v>
       </c>
@@ -9792,10 +9801,10 @@
       <c r="D312" s="19"/>
       <c r="E312" s="22"/>
       <c r="F312" s="21" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="313" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
         <v>374</v>
       </c>
@@ -9807,13 +9816,13 @@
       </c>
       <c r="D313" s="24"/>
       <c r="E313" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F313" s="23" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A314" s="2" t="s">
         <v>374</v>
       </c>
@@ -9827,13 +9836,16 @@
         <v>375</v>
       </c>
       <c r="E314" s="4" t="s">
-        <v>845</v>
+        <v>862</v>
       </c>
       <c r="G314" s="70" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="315" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H314" s="2" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A315" s="21" t="s">
         <v>375</v>
       </c>
@@ -9851,7 +9863,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
         <v>375</v>
       </c>
@@ -9909,7 +9921,7 @@
         <v>109</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -9981,10 +9993,10 @@
         <v>109</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -9995,10 +10007,10 @@
         <v>109</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -10009,10 +10021,10 @@
         <v>109</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -10023,10 +10035,10 @@
         <v>109</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -10154,7 +10166,7 @@
         <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>763</v>
@@ -10168,7 +10180,7 @@
         <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>763</v>
@@ -10184,7 +10196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -10196,74 +10208,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B1" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B3" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B4" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="B5" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B6" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>859</v>
+      </c>
+      <c r="B7" t="s">
         <v>861</v>
-      </c>
-      <c r="B7" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B8" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="B9" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10316,18 +10328,18 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B16" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10615,7 +10627,7 @@
         <v>676</v>
       </c>
       <c r="B53" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -10628,10 +10640,10 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>814</v>
+      </c>
+      <c r="B55" t="s">
         <v>815</v>
-      </c>
-      <c r="B55" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -10772,7 +10784,7 @@
         <v>667</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -10786,7 +10798,7 @@
         <v>748</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -10800,7 +10812,7 @@
         <v>673</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -10814,7 +10826,7 @@
         <v>668</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -10831,7 +10843,7 @@
         <v>747</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -10845,7 +10857,7 @@
         <v>749</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -10916,7 +10928,7 @@
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F13" s="21" t="s">
         <v>672</v>
@@ -11049,7 +11061,7 @@
         <v>662</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -11083,12 +11095,12 @@
         <v>662</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>100</v>
@@ -11098,52 +11110,52 @@
       </c>
       <c r="D24" s="19"/>
       <c r="E24" s="22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>805</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="E25" s="83" t="s">
+        <v>817</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>806</v>
-      </c>
-      <c r="E25" s="83" t="s">
-        <v>818</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>808</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>809</v>
-      </c>
       <c r="E26" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>100</v>
@@ -11153,31 +11165,31 @@
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="22" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D28" s="24"/>
       <c r="E28" s="34"/>
       <c r="F28" s="23" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>100</v>
@@ -11186,10 +11198,10 @@
         <v>199</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
   </sheetData>
@@ -11236,7 +11248,7 @@
         <v>109</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
   </sheetData>
@@ -11249,7 +11261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G316"/>
   <sheetViews>
-    <sheetView topLeftCell="A286" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
       <selection activeCell="E315" sqref="E315"/>
     </sheetView>
   </sheetViews>
@@ -11316,12 +11328,12 @@
         <v>100</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D3" s="86"/>
       <c r="E3" s="34"/>
       <c r="F3" s="25" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G3" s="23"/>
     </row>
@@ -11382,10 +11394,10 @@
         <v>100</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>790</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>791</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -11764,7 +11776,7 @@
         <v>108</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F30" s="80" t="s">
         <v>95</v>
@@ -11850,7 +11862,7 @@
         <v>735</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -11867,7 +11879,7 @@
         <v>736</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -11887,7 +11899,7 @@
         <v>587</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -11907,7 +11919,7 @@
         <v>588</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>208</v>
@@ -12019,7 +12031,7 @@
         <v>100</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>696</v>
@@ -12135,7 +12147,7 @@
         <v>100</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>447</v>
@@ -12159,7 +12171,7 @@
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="22" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F53" s="21" t="s">
         <v>756</v>
@@ -12189,7 +12201,7 @@
         <v>100</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D55" s="24"/>
       <c r="E55" s="34"/>
@@ -12267,12 +12279,12 @@
         <v>100</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D60" s="24"/>
       <c r="E60" s="34"/>
       <c r="F60" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -12446,18 +12458,18 @@
         <v>453</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>532</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="21" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B72" s="21" t="s">
         <v>100</v>
@@ -12468,12 +12480,12 @@
       <c r="D72" s="19"/>
       <c r="E72" s="22"/>
       <c r="F72" s="21" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>100</v>
@@ -12614,7 +12626,7 @@
         <v>738</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -12631,7 +12643,7 @@
         <v>737</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -12651,7 +12663,7 @@
         <v>589</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -12671,7 +12683,7 @@
         <v>590</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>208</v>
@@ -12783,7 +12795,7 @@
         <v>100</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>696</v>
@@ -12899,7 +12911,7 @@
         <v>100</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>194</v>
@@ -12923,7 +12935,7 @@
       </c>
       <c r="D99" s="19"/>
       <c r="E99" s="22" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F99" s="21" t="s">
         <v>756</v>
@@ -12953,7 +12965,7 @@
         <v>100</v>
       </c>
       <c r="C101" s="23" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D101" s="24"/>
       <c r="E101" s="34"/>
@@ -13020,7 +13032,7 @@
       <c r="D105" s="24"/>
       <c r="E105" s="34"/>
       <c r="F105" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="106" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -13031,12 +13043,12 @@
         <v>100</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D106" s="24"/>
       <c r="E106" s="34"/>
       <c r="F106" s="23" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="107" spans="1:6" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -13210,18 +13222,18 @@
         <v>393</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>531</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="118" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="21" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B118" s="21" t="s">
         <v>100</v>
@@ -13232,12 +13244,12 @@
       <c r="D118" s="19"/>
       <c r="E118" s="22"/>
       <c r="F118" s="21" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>100</v>
@@ -13361,7 +13373,7 @@
     </row>
     <row r="127" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="21" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B127" s="21" t="s">
         <v>100</v>
@@ -13371,15 +13383,15 @@
       </c>
       <c r="D127" s="19"/>
       <c r="E127" s="22" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F127" s="21" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="128" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="25" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B128" s="25" t="s">
         <v>100</v>
@@ -13389,7 +13401,7 @@
       </c>
       <c r="E128" s="85"/>
       <c r="F128" s="25" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -13404,10 +13416,10 @@
       </c>
       <c r="D129" s="19"/>
       <c r="E129" s="22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F129" s="21" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -13719,7 +13731,7 @@
         <v>725</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="149" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -13735,7 +13747,7 @@
       <c r="D149" s="19"/>
       <c r="E149" s="22"/>
       <c r="F149" s="21" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.2">
@@ -13775,7 +13787,7 @@
         <v>539</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G151" s="68" t="s">
         <v>366</v>
@@ -14121,7 +14133,7 @@
         <v>726</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="172" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -14137,7 +14149,7 @@
       <c r="D172" s="19"/>
       <c r="E172" s="22"/>
       <c r="F172" s="21" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
@@ -14177,7 +14189,7 @@
         <v>540</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G174" s="68" t="s">
         <v>366</v>
@@ -14609,7 +14621,7 @@
         <v>413</v>
       </c>
       <c r="E199" s="34" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F199" s="23" t="s">
         <v>608</v>
@@ -14682,7 +14694,7 @@
         <v>419</v>
       </c>
       <c r="E203" s="34" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F203" s="23" t="s">
         <v>648</v>
@@ -14840,7 +14852,7 @@
         <v>418</v>
       </c>
       <c r="E212" s="34" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F212" s="23" t="s">
         <v>649</v>
@@ -15059,7 +15071,7 @@
         <v>241</v>
       </c>
       <c r="E225" s="34" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F225" s="23" t="s">
         <v>608</v>
@@ -15132,7 +15144,7 @@
         <v>239</v>
       </c>
       <c r="E229" s="34" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F229" s="23" t="s">
         <v>648</v>
@@ -15288,7 +15300,7 @@
         <v>243</v>
       </c>
       <c r="E238" s="34" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F238" s="23" t="s">
         <v>649</v>
@@ -15965,7 +15977,7 @@
         <v>369</v>
       </c>
       <c r="E280" s="4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F280" s="2" t="s">
         <v>351</v>
@@ -16070,7 +16082,7 @@
         <v>369</v>
       </c>
       <c r="E286" s="48" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="287" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.2">
@@ -16324,7 +16336,7 @@
         <v>364</v>
       </c>
       <c r="E302" s="4" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F302" s="2" t="s">
         <v>351</v>
@@ -16477,7 +16489,7 @@
         <v>374</v>
       </c>
       <c r="E311" s="4" t="s">
-        <v>768</v>
+        <v>865</v>
       </c>
       <c r="G311" s="70" t="s">
         <v>377</v>
@@ -16496,7 +16508,7 @@
       <c r="D312" s="19"/>
       <c r="E312" s="22"/>
       <c r="F312" s="21" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="313" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.2">
@@ -16511,10 +16523,10 @@
       </c>
       <c r="D313" s="24"/>
       <c r="E313" s="34" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F313" s="23" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.2">
@@ -16531,7 +16543,7 @@
         <v>375</v>
       </c>
       <c r="E314" s="4" t="s">
-        <v>845</v>
+        <v>862</v>
       </c>
       <c r="G314" s="70" t="s">
         <v>377</v>
@@ -16613,7 +16625,7 @@
         <v>109</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -16685,10 +16697,10 @@
         <v>109</v>
       </c>
       <c r="C8" s="65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -16699,10 +16711,10 @@
         <v>109</v>
       </c>
       <c r="C9" s="65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -16713,10 +16725,10 @@
         <v>109</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -16727,10 +16739,10 @@
         <v>109</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -16858,7 +16870,7 @@
         <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>763</v>
@@ -16872,7 +16884,7 @@
         <v>109</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>763</v>

</xml_diff>